<commit_message>
Updated requirements for images and albums
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MovieDbCode\MovieDb\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="113">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -278,9 +273,6 @@
     </r>
   </si>
   <si>
-    <t>8,9</t>
-  </si>
-  <si>
     <r>
       <t>Create reviews table: reviews(</t>
     </r>
@@ -472,6 +464,159 @@
   </si>
   <si>
     <t>Create Form for creating lists based on movie or person and the title of the list</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <r>
+      <t>Create images table: images(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, name, path, extension, description)</t>
+    </r>
+  </si>
+  <si>
+    <t>20, 21, 22, 23</t>
+  </si>
+  <si>
+    <t>21, 22,23</t>
+  </si>
+  <si>
+    <r>
+      <t>Create albums table: albums(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id)</t>
+    </r>
+  </si>
+  <si>
+    <t>21, 22, 23</t>
+  </si>
+  <si>
+    <t>49, 50</t>
+  </si>
+  <si>
+    <t>Many-to-Many relationship between images and albums -- Create pivot table: album_image(album_id, image_id) : album_id references id on albums, image_id references id on images</t>
+  </si>
+  <si>
+    <t>8, 9</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>38, 49</t>
+  </si>
+  <si>
+    <t>One-to-One relationship from users to images to support avatars</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>49, 53</t>
+  </si>
+  <si>
+    <t>The name of the image is unique and randomly generated</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Images are partitioned into directories, with a maximum of 1000 images per directory. Images are placed into directories based on their id in the database. I.e. 0-999, 1000-1999, 2000-2999, … will each reside in a separate directory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57 </t>
+  </si>
+  <si>
+    <t>Supported image formats are png, jpg, and bmp.</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>The name, public path, and absolute file path of the image should be retrievable.</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>Image file is stored in the file system and associated with a single record in the database. Images can be retrieved using the path / name / extension in the record.</t>
+  </si>
+  <si>
+    <t>49, 53, 55, 56</t>
+  </si>
+  <si>
+    <t>An image record should be created if and only if a corresponding image file is created in the correct directory.</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Deleting an image record should also attemp to delete the corresponding image file. If the image file is non-existent, the record should still be removed.</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>Albums</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Image model with one-to-one relationship to User and many-to-many relationship with Album</t>
+  </si>
+  <si>
+    <t>Album model with a many-to-many relationship with Image</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>50, 61</t>
+  </si>
+  <si>
+    <t>Ability to add an image to an album or remove an image from an album.</t>
   </si>
 </sst>
 </file>
@@ -515,11 +660,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +726,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,7 +761,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -824,32 +970,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E52"/>
+  <dimension ref="A4:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="176.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
@@ -857,13 +1003,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
@@ -871,13 +1017,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
@@ -885,13 +1031,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
@@ -899,13 +1045,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
@@ -913,13 +1059,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="2">
         <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
@@ -927,13 +1073,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="2">
         <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
@@ -941,13 +1087,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>6</v>
       </c>
       <c r="E11" t="s">
@@ -955,13 +1101,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="2">
         <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
@@ -969,13 +1115,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="B13" s="2">
         <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
@@ -983,13 +1129,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="2">
         <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E14" t="s">
@@ -997,13 +1143,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="2">
         <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>8</v>
       </c>
       <c r="E15" t="s">
@@ -1011,13 +1157,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="2">
         <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>11</v>
       </c>
       <c r="E16" t="s">
@@ -1025,13 +1171,13 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="2">
         <v>13</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>11</v>
       </c>
       <c r="E17" t="s">
@@ -1039,13 +1185,13 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="B18" s="2">
         <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>11</v>
       </c>
       <c r="E18" t="s">
@@ -1053,13 +1199,13 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="B19" s="2">
         <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>13</v>
       </c>
       <c r="E19" t="s">
@@ -1067,13 +1213,13 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20">
+      <c r="B20" s="2">
         <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
@@ -1081,13 +1227,13 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21">
+      <c r="B21" s="2">
         <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
@@ -1095,13 +1241,13 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="B22" s="2">
         <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
@@ -1109,13 +1255,13 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="B23" s="2">
         <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -1123,13 +1269,13 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="B24" s="2">
         <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="s">
@@ -1137,13 +1283,13 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25">
+      <c r="B25" s="2">
         <v>21</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
@@ -1151,13 +1297,13 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="B26" s="2">
         <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E26" t="s">
@@ -1165,13 +1311,13 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27">
+      <c r="B27" s="2">
         <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E27" t="s">
@@ -1179,13 +1325,13 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28">
+      <c r="B28" s="2">
         <v>24</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
@@ -1193,13 +1339,13 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29">
+      <c r="B29" s="2">
         <v>25</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>6</v>
       </c>
       <c r="E29" t="s">
@@ -1207,13 +1353,13 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30">
+      <c r="B30" s="2">
         <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1221,13 +1367,13 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31">
+      <c r="B31" s="2">
         <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E31" t="s">
@@ -1235,13 +1381,13 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32">
+      <c r="B32" s="2">
         <v>28</v>
       </c>
       <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E32" t="s">
@@ -1249,13 +1395,13 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33">
+      <c r="B33" s="2">
         <v>29</v>
       </c>
       <c r="C33" t="s">
         <v>46</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E33" t="s">
@@ -1263,13 +1409,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="B34" s="2">
         <v>30</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E34" t="s">
@@ -1277,13 +1423,13 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35">
+      <c r="B35" s="2">
         <v>31</v>
       </c>
       <c r="C35" t="s">
         <v>46</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E35" t="s">
@@ -1291,13 +1437,13 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36">
+      <c r="B36" s="2">
         <v>32</v>
       </c>
       <c r="C36" t="s">
         <v>46</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>6</v>
       </c>
       <c r="E36" t="s">
@@ -1305,16 +1451,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="2">
         <v>16</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>33</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E37" t="s">
@@ -1322,16 +1468,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>17</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>34</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E38" t="s">
@@ -1339,16 +1485,16 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>17</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>35</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E39" t="s">
@@ -1356,16 +1502,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>17</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>36</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E40" t="s">
@@ -1373,16 +1519,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>6</v>
-      </c>
-      <c r="B41">
+      <c r="A41" s="2">
+        <v>6</v>
+      </c>
+      <c r="B41" s="2">
         <v>37</v>
       </c>
       <c r="C41" t="s">
         <v>58</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E41" t="s">
@@ -1390,16 +1536,16 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>3</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>38</v>
       </c>
       <c r="C42" t="s">
         <v>58</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" t="s">
@@ -1407,16 +1553,16 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>5</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>39</v>
       </c>
       <c r="C43" t="s">
         <v>58</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
@@ -1424,149 +1570,390 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44">
+      <c r="A44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="2">
         <v>40</v>
       </c>
       <c r="C44" t="s">
         <v>58</v>
       </c>
-      <c r="D44" t="s">
-        <v>69</v>
+      <c r="D44" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>10</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>41</v>
       </c>
       <c r="C45" t="s">
         <v>58</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="2">
         <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>18</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>42</v>
       </c>
       <c r="C46" t="s">
         <v>58</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>6</v>
-      </c>
-      <c r="B47">
+      <c r="A47" s="2">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2">
         <v>43</v>
       </c>
       <c r="C47" t="s">
         <v>58</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>6</v>
-      </c>
-      <c r="B48">
+      <c r="A48" s="2">
+        <v>6</v>
+      </c>
+      <c r="B48" s="2">
         <v>44</v>
       </c>
       <c r="C48" t="s">
         <v>58</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" t="s">
         <v>67</v>
       </c>
-      <c r="E48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
         <v>45</v>
       </c>
       <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
         <v>70</v>
       </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>46</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>46</v>
-      </c>
-      <c r="C50" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>48</v>
+      </c>
+      <c r="C52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="2">
+        <v>49</v>
+      </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="2">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="2">
+        <v>51</v>
+      </c>
+      <c r="C55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>47</v>
-      </c>
-      <c r="C51" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>48</v>
-      </c>
-      <c r="C52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" t="s">
-        <v>73</v>
+      <c r="D57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" t="s">
+        <v>106</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A56:B56" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated user stories and functional reqs. for user pages
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MovieDbCode\MovieDb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="127">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -138,9 +143,6 @@
     <t>Create default favorite movies list on account creation.</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Make a clickable button to create lists on user page. Have the ability to title the list and select the type (movie, person).</t>
   </si>
   <si>
@@ -617,6 +619,51 @@
   </si>
   <si>
     <t>Ability to add an image to an album or remove an image from an album.</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Ability to delete a movie list from the movie list view tab</t>
+  </si>
+  <si>
+    <t>Ability to delete a people list from the people list view tab</t>
+  </si>
+  <si>
+    <t>Ability to delete a particular movie from a movie list</t>
+  </si>
+  <si>
+    <t>Ability to delete a particular person from a person list</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>Ability to add a movie to a movie list from within the movie list tab</t>
+  </si>
+  <si>
+    <t>Abilility to add a person to a person list from within the person list tab</t>
   </si>
 </sst>
 </file>
@@ -726,7 +773,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,7 +808,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -970,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E66"/>
+  <dimension ref="A4:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +1034,7 @@
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1360,10 +1407,10 @@
         <v>38</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1374,10 +1421,10 @@
         <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1388,10 +1435,10 @@
         <v>16</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,13 +1446,13 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" t="s">
         <v>46</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1413,13 +1460,13 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1427,13 +1474,13 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1441,13 +1488,13 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="2">
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1458,13 +1505,13 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
         <v>53</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1545,7 @@
         <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,7 +1562,7 @@
         <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1526,13 +1573,13 @@
         <v>37</v>
       </c>
       <c r="C41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
         <v>58</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1543,13 +1590,13 @@
         <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1560,30 +1607,30 @@
         <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" s="2">
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,13 +1641,13 @@
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="2">
         <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1611,13 +1658,13 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1628,13 +1675,13 @@
         <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1645,13 +1692,13 @@
         <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
         <v>66</v>
-      </c>
-      <c r="E48" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,13 +1706,13 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
         <v>69</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1673,13 +1720,13 @@
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1687,13 +1734,13 @@
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,251 +1748,353 @@
         <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2">
         <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B54" s="2">
         <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55" s="2">
         <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E55" t="s">
         <v>80</v>
-      </c>
-      <c r="E55" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C56" t="s">
-        <v>58</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C57" t="s">
-        <v>74</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="E57" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C58" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C60" t="s">
-        <v>74</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C61" t="s">
-        <v>74</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C64" t="s">
-        <v>74</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" t="s">
         <v>105</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E65" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C66" t="s">
-        <v>106</v>
-      </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E66" s="2" t="s">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>112</v>
+      </c>
+      <c r="C67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C71" t="s">
+        <v>68</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" t="s">
+        <v>68</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding manual testing scripts
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="238">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -837,16 +837,10 @@
     <t>28</t>
   </si>
   <si>
-    <t>For menu bar searching, each word considered as a separate search term, and a result must match all of the given terms. For instance the string 'return king' would match 'The Return of the King', but not 'Return of the Jedi'.</t>
-  </si>
-  <si>
     <t>Menu bar search can find results for partial matches. For instance 'kellen' should match 'Ian McKellen'.</t>
   </si>
   <si>
     <t>96</t>
-  </si>
-  <si>
-    <t>Search pane in the menu bar that offers suggestions in a drop-down. Movies and people results are both displayed as suggestions.</t>
   </si>
   <si>
     <t>Menu bar searching should be done asynchronously, requiring a RESTful API that can return search results based on a search term.</t>
@@ -946,9 +940,6 @@
     <t>The name an person is known by should be the name displayed on the website. If an person has a name they are known as, other than their given name, that should be their 'alias'</t>
   </si>
   <si>
-    <t>Menu bar search displays a thumbnail of the default image associated with the search result. Results that have no default image display some placeholder image. Year of birth and year of death are displayed for people. Release year is displayed for movies</t>
-  </si>
-  <si>
     <t>Movie</t>
   </si>
   <si>
@@ -1053,6 +1044,21 @@
   </si>
   <si>
     <t>Each user has an avatar, which is null by default. The avatar can be changed, or set to null.</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>Movies and people results are both displayed as suggestions in the menu bar search.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search pane in the menu bar that offers suggestions in a drop-down. </t>
+  </si>
+  <si>
+    <t>Menu bar search displays a thumbnail of the default image associated with the search result. Results that have no default image display some placeholder image. Year of birth and year of death are displayed for people. Release year is displayed for movies.</t>
+  </si>
+  <si>
+    <t>For menu bar searching, each word considered as a separate search term, and a result must match all of the given terms. For instance the string 'return king' would match 'The Return of the King', but not 'Return of the Jedi'. Words surrounded by double quotes should be considered as a single word, and the result must match the entire string inside of the double quotes.</t>
   </si>
 </sst>
 </file>
@@ -1464,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,22 +1488,22 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1522,20 +1528,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="7">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1842,7 +1848,7 @@
     <row r="38" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>4</v>
@@ -2272,7 +2278,7 @@
         <v>6</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2476,7 +2482,7 @@
         <v>107</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2598,20 +2604,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="12" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2649,20 +2655,20 @@
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="88" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2697,7 +2703,7 @@
         <v>180</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2768,20 +2774,20 @@
         <v>153</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2921,20 +2927,20 @@
         <v>166</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E104" s="2" t="s">
+      <c r="E104" s="3" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2972,72 +2978,72 @@
         <v>172</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D107" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+      <c r="E107" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D108" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+      <c r="E108" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="2" t="s">
+      <c r="D109" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" s="3" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C110" t="s">
-        <v>4</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3045,7 +3051,7 @@
         <v>182</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>4</v>
@@ -3054,7 +3060,7 @@
         <v>185</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3062,7 +3068,7 @@
         <v>123</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>102</v>
@@ -3071,7 +3077,7 @@
         <v>185</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3079,7 +3085,7 @@
         <v>182</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>71</v>
@@ -3088,15 +3094,15 @@
         <v>86</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>102</v>
@@ -3105,24 +3111,24 @@
         <v>107</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="115" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B115" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D115" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C115" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="E115" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3130,16 +3136,16 @@
         <v>129</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C116" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3147,16 +3153,16 @@
         <v>129</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3164,7 +3170,7 @@
         <v>189</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>4</v>
@@ -3173,7 +3179,7 @@
         <v>6</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3181,7 +3187,7 @@
         <v>189</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>4</v>
@@ -3190,7 +3196,7 @@
         <v>6</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3198,16 +3204,16 @@
         <v>189</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3215,16 +3221,16 @@
         <v>189</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3232,16 +3238,33 @@
         <v>79</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D122" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-adding overwritten requirements from chris
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="296">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -1059,6 +1059,180 @@
   </si>
   <si>
     <t>For menu bar searching, each word considered as a separate search term, and a result must match all of the given terms. For instance the string 'return king' would match 'The Return of the King', but not 'Return of the Jedi'. Words surrounded by double quotes should be considered as a single word, and the result must match the entire string inside of the double quotes.</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>A review can be created for any existing movie through a review creation page.</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>The user must be logged in to create a review.</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>The user can enter a title, movie rating, and review body when creating a review.</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>A new review can be submitted by clicking the submit button on the create review page.</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>A specific review's contents can be displayed on a page.</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>The display review page shows the related movie title.</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>The display review page shows the review title, and review body.</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>The display review page shows the review movie rating using star images.</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>The display review page has a user information section.</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>The user information section displays a user's username, avatar, and when the review was posted.</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>The user information section contains buttons for deleting and editing a review.</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>The delete and edit buttons in the user info section only display for the owning user and comment or review moderators.</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>A comment button is displayed and takes user to a comment creation page when clicked.</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>The comment button is only displayed when the user is logged in.</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Upvote and downvote buttons are displayed on the review display page.</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>The review's score is displayed on the review display page.</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>Clicking the upvote or downvote buttons while not logged in displays an error popup.</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>123,124</t>
+  </si>
+  <si>
+    <t>Clicking on the upvote or downvote button reflects in the review score.</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>123, 124</t>
+  </si>
+  <si>
+    <t>Clicking on the upvote or downvote button sends an ajax request to the server to increment or decrement the review score.</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>Clicking on an already selected upvote or downvote button revokes the user's vote through an AJAX call.</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>Comments associated with a review are displayed under the review on the review display page.</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>A comment displays its body.</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>A comment has a user section that displays the user's username, avatar, and comment post date.</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>Edit and delete buttons are displayed in the comment's user section.</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>The edit and delete buttons for comments only display for the user who created them, and for comment or review moderators.</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>The delete button for a review sends an ajax request to have the review deleted, and then refreshes the page.</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>If a user attempts to create a review for a non existant movie, a movie not found page is displayed.</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>If a user attempts to display a review that does no exist, a review not found page is displayed.</t>
   </si>
 </sst>
 </file>
@@ -1470,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3265,6 +3439,386 @@
       </c>
       <c r="E123" s="3" t="s">
         <v>234</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C124" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C125" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E125" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B126" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C126" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E126" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C127" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E127" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B128" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C128" t="s">
+        <v>15</v>
+      </c>
+      <c r="E128" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C129" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E129" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C130" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E130" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C131" t="s">
+        <v>15</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E131" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C132" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E132" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C133" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E133" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C134" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E134" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C135" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E135" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B136" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E136" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B137" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C137" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E137" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C138" t="s">
+        <v>15</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E138" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C139" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E139" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C140" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E140" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C141" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E141" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B142" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C142" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E142" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B143" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C143" t="s">
+        <v>15</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E143" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B144" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C144" t="s">
+        <v>15</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E144" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C145" t="s">
+        <v>15</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E145" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C146" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E146" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C147" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E147" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C148" t="s">
+        <v>15</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E148" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C149" t="s">
+        <v>15</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E149" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C150" t="s">
+        <v>15</v>
+      </c>
+      <c r="E150" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C151" t="s">
+        <v>15</v>
+      </c>
+      <c r="E151" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Administration functional requirements. Can now begin testing.
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MovieDbCode\MovieDb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="302">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -93,28 +98,10 @@
     <t>Receive a notification when a user comments on a review.</t>
   </si>
   <si>
-    <t>Central administration page that displays options for creating Movies or People.</t>
-  </si>
-  <si>
     <t>View and Controller for displaying associated person info, i.e. What roles they've had in movies, and other biographic information. Links for admin to Edit or Delete person.</t>
   </si>
   <si>
     <t>View and Controller for displaying associated movie info. Reviews and comments are displayed on the page below the movie info. Links for admin to Edit or Delete movie.</t>
-  </si>
-  <si>
-    <t>Page to create a Person. Form has all fields for person info. Form should also be able to upload a picture.</t>
-  </si>
-  <si>
-    <t>Page to create a Movie. Form has fields for all movie info. Form should also be able to upload a picture.</t>
-  </si>
-  <si>
-    <t>Page to edit a Person. Form has all fields for person info that are autopopulated with corresponding person. Form should also be able to change picture associated.</t>
-  </si>
-  <si>
-    <t>Page to edit a Movie. Form has all fields for movie info that are autopopulated with corresponding movie. Form should also be able to change picture associated.</t>
-  </si>
-  <si>
-    <t>Controller that properly deletes a movie, and all corresponding movie information from the database. Includes reviews, and discussions.</t>
   </si>
   <si>
     <t>Controller that properly deletes a person, and all corresponding person information from the database.</t>
@@ -1234,12 +1221,48 @@
   <si>
     <t>If a user attempts to display a review that does no exist, a review not found page is displayed.</t>
   </si>
+  <si>
+    <t>TESTING IN PROGRESS</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Central administration page that displays options for creating Movies, People, Characters (option to show all movies, option to show all people).</t>
+  </si>
+  <si>
+    <t>Page to create a Movie. Form has fields for all movie info (title, country, release date, genre, rating, runtime, synopsis).</t>
+  </si>
+  <si>
+    <t>Page to edit a Movie. Form has all fields for movie info that are autopopulated with corresponding movie.  Form should also be able to upload an image Form should also be able to change associated images.</t>
+  </si>
+  <si>
+    <t>Page to edit a Person. Form has all fields for person info that are autopopulated with corresponding person. Form should also be able to upload an image Form should also be able to change associated images.</t>
+  </si>
+  <si>
+    <t>Page to create a Person. Form has all fields for person info (first name, middle name, last name, first alias, middle alias, last alias, country of birth, date of birth, date of death, biography).</t>
+  </si>
+  <si>
+    <t>Controller that properly deletes a movie, and all corresponding movie information from the database (includes reviews, and discussions).</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Page to create a Character. Form has all fields for character info (character name, character bio).</t>
+  </si>
+  <si>
+    <t>18.5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1269,8 +1292,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1301,8 +1331,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1310,11 +1346,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1331,8 +1383,17 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1400,7 +1461,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1435,7 +1496,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1644,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,32 +1723,37 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="15" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1704,7 +1770,7 @@
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -1721,7 +1787,7 @@
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1730,15 +1796,15 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -1747,10 +1813,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,7 +1886,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1834,7 +1900,7 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1921,123 +1987,146 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
+    <row r="31" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="B31" s="18">
         <v>16</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
+      <c r="E31" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B32" s="16">
         <v>17</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
+      <c r="E32" s="15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B33" s="16">
         <v>18</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
+      <c r="E33" s="15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B35" s="16">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
+      <c r="D35" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" s="16">
         <v>20</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
+      <c r="D36" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B37" s="16">
         <v>21</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
+      <c r="D37" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B38" s="16">
         <v>22</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>34</v>
+      <c r="D38" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
-        <v>123</v>
+        <v>204</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>4</v>
@@ -2046,153 +2135,151 @@
         <v>6</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="2">
-        <v>25</v>
-      </c>
-      <c r="C40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E40" t="s">
-        <v>37</v>
+      <c r="E40" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="2">
         <v>6</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>38</v>
+      <c r="E41" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E43" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E46" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
         <v>32</v>
       </c>
-      <c r="C47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="2">
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" s="2">
         <v>6</v>
       </c>
-      <c r="E47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>16</v>
-      </c>
-      <c r="B48" s="2">
-        <v>33</v>
-      </c>
-      <c r="C48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E48" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>17</v>
-      </c>
-      <c r="B49" s="2">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="B49" s="20">
+        <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2200,7 +2287,7 @@
         <v>17</v>
       </c>
       <c r="B50" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -2209,7 +2296,7 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2217,7 +2304,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
@@ -2226,126 +2313,126 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>17</v>
+      </c>
+      <c r="B52" s="2">
+        <v>36</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="7">
-        <v>37</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>56</v>
+      <c r="E52" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B53" s="7">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B54" s="7">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>78</v>
+      <c r="A55" s="7">
+        <v>5</v>
       </c>
       <c r="B55" s="7">
+        <v>39</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="7">
         <v>40</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" s="8" t="s">
+      <c r="C56" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
-        <v>10</v>
-      </c>
-      <c r="B56" s="7">
-        <v>41</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D56" s="7">
-        <v>40</v>
-      </c>
       <c r="E56" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B57" s="7">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>6</v>
+        <v>49</v>
+      </c>
+      <c r="D57" s="7">
+        <v>40</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B58" s="7">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2353,140 +2440,140 @@
         <v>6</v>
       </c>
       <c r="B59" s="7">
+        <v>43</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>6</v>
+      </c>
+      <c r="B60" s="7">
         <v>44</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="2">
-        <v>45</v>
-      </c>
-      <c r="C60" t="s">
-        <v>66</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" t="s">
-        <v>67</v>
+      <c r="C60" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" s="7">
-        <v>49</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="8" t="s">
-        <v>72</v>
+      <c r="E64" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B65" s="7">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>200</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B66" s="7">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>80</v>
+        <v>69</v>
+      </c>
+      <c r="B67" s="7">
+        <v>51</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>82</v>
+        <v>70</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2494,64 +2581,64 @@
         <v>73</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>96</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>90</v>
@@ -2559,656 +2646,656 @@
     </row>
     <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D73" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E77" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E75" s="3" t="s">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="7" t="s">
+      <c r="C78" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C78" t="s">
-        <v>66</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>114</v>
+      <c r="E78" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C79" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C81" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="C82" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D82" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C83" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>125</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C84" t="s">
+        <v>60</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E85" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>134</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E88" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>235</v>
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>4</v>
@@ -3217,151 +3304,151 @@
         <v>6</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>185</v>
+        <v>6</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>123</v>
+        <v>176</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>207</v>
+        <v>96</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>211</v>
+        <v>101</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C117" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>207</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E118" s="7" t="s">
-        <v>221</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>4</v>
@@ -3370,455 +3457,472 @@
         <v>6</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C120" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C120" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D120" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>229</v>
+      <c r="D120" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>182</v>
+        <v>73</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C123" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C124" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C124" t="s">
-        <v>15</v>
-      </c>
-      <c r="E124" t="s">
-        <v>239</v>
+      <c r="D124" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C125" t="s">
         <v>15</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="E125" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C126" t="s">
         <v>15</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E126" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C127" t="s">
         <v>15</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E127" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C128" t="s">
         <v>15</v>
       </c>
+      <c r="D128" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="E128" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C129" t="s">
         <v>15</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E129" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C130" t="s">
         <v>15</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E130" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C131" t="s">
         <v>15</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E131" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C132" t="s">
         <v>15</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E132" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C133" t="s">
         <v>15</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="E133" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C134" t="s">
         <v>15</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E134" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C135" t="s">
         <v>15</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="E135" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C136" t="s">
         <v>15</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E136" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C137" t="s">
         <v>15</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E137" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C138" t="s">
         <v>15</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E138" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C139" t="s">
         <v>15</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E139" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C140" t="s">
         <v>15</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="E140" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C141" t="s">
         <v>15</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="E141" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C142" t="s">
         <v>15</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="E142" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="2" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C143" t="s">
         <v>15</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E143" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C144" t="s">
         <v>15</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="E144" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E145" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C146" t="s">
         <v>15</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>282</v>
+        <v>248</v>
       </c>
       <c r="E146" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C147" t="s">
         <v>15</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E147" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C148" t="s">
         <v>15</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E148" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C149" t="s">
         <v>15</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="E149" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B150" s="2" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C150" t="s">
         <v>15</v>
       </c>
+      <c r="D150" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="E150" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="C151" t="s">
         <v>15</v>
       </c>
       <c r="E151" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B152" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C152" t="s">
+        <v>15</v>
+      </c>
+      <c r="E152" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started testing the admin controller and updated functional requirements once again. I am having a problem with my views and testing. In order to get my test to pass successfully, I have to comment out the errors portion of my blade views. I left them commented out for now (can be seen in the commit) but I need to find a solution for this. I have been on google but haven't been able to find a working solution. I will continue writing the rest of my tests throughout the weekend.
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1366,7 +1366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1387,10 +1387,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1708,7 +1712,7 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,71 +1991,71 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="20">
         <v>16</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="21" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="23">
         <v>17</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="25" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="23">
         <v>18</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="25" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="25" t="s">
         <v>299</v>
       </c>
     </row>
@@ -2269,7 +2273,7 @@
       <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B49" s="18">
         <v>33</v>
       </c>
       <c r="C49" t="s">

</xml_diff>

<commit_message>
Changed reqs, will push testing soon
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MovieDbCode\MovieDb\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="306">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -1051,9 +1046,6 @@
     <t>109</t>
   </si>
   <si>
-    <t>A review can be created for any existing movie through a review creation page.</t>
-  </si>
-  <si>
     <t>110</t>
   </si>
   <si>
@@ -1111,9 +1103,6 @@
     <t>119</t>
   </si>
   <si>
-    <t>The user information section contains buttons for deleting and editing a review.</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
@@ -1256,13 +1245,31 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>A user can only create one review per movie.</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>The delete review button deletes a review, as well as the comments and votes associated with it.</t>
+  </si>
+  <si>
+    <t>A review creation page exists which is used to create reviews.</t>
+  </si>
+  <si>
+    <t>The user information section contains buttons for deleting and editing a review when the user is logged in.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1299,8 +1306,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1337,6 +1351,17 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FF99"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1362,11 +1387,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1395,9 +1421,14 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1465,7 +1496,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1497,10 +1528,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1532,7 +1562,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1708,14 +1737,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E152"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1724,38 +1753,38 @@
     <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="E2" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="E3" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="E4" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="E5" s="9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="E6" s="15" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1772,7 +1801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="8" customFormat="1">
       <c r="A16" s="7" t="s">
         <v>130</v>
       </c>
@@ -1789,7 +1818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="4" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>131</v>
       </c>
@@ -1806,7 +1835,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="4" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>132</v>
       </c>
@@ -1823,7 +1852,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -1837,7 +1866,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -1851,7 +1880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -1865,7 +1894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -1879,7 +1908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="B23" s="2">
         <v>8</v>
       </c>
@@ -1893,7 +1922,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -1907,7 +1936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -1921,7 +1950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -1935,7 +1964,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -1949,7 +1978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -1963,7 +1992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -1977,7 +2006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -1991,9 +2020,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="21" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B31" s="20">
         <v>16</v>
@@ -2005,12 +2034,12 @@
         <v>6</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="24" customFormat="1">
       <c r="A32" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B32" s="23">
         <v>17</v>
@@ -2022,12 +2051,12 @@
         <v>6</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="24" customFormat="1">
       <c r="A33" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B33" s="23">
         <v>18</v>
@@ -2039,15 +2068,15 @@
         <v>6</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="24" customFormat="1">
       <c r="A34" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>16</v>
@@ -2056,12 +2085,12 @@
         <v>6</v>
       </c>
       <c r="E34" s="25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="24" customFormat="1">
+      <c r="A35" s="22" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>301</v>
       </c>
       <c r="B35" s="23">
         <v>19</v>
@@ -2070,15 +2099,15 @@
         <v>16</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="24" customFormat="1">
       <c r="A36" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B36" s="23">
         <v>20</v>
@@ -2087,15 +2116,15 @@
         <v>16</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1">
       <c r="A37" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B37" s="16">
         <v>21</v>
@@ -2107,12 +2136,12 @@
         <v>106</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="14" customFormat="1">
       <c r="A38" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B38" s="16">
         <v>22</v>
@@ -2127,7 +2156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="9" customFormat="1">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>204</v>
@@ -2142,7 +2171,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="9" customFormat="1">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>117</v>
@@ -2157,7 +2186,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="B41" s="2">
         <v>25</v>
       </c>
@@ -2171,7 +2200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="B42" s="2">
         <v>26</v>
       </c>
@@ -2185,7 +2214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2199,7 +2228,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2213,7 +2242,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="B45" s="2">
         <v>29</v>
       </c>
@@ -2227,7 +2256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="B46" s="2">
         <v>30</v>
       </c>
@@ -2241,7 +2270,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="B47" s="2">
         <v>31</v>
       </c>
@@ -2255,7 +2284,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="B48" s="2">
         <v>32</v>
       </c>
@@ -2269,7 +2298,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="2">
         <v>16</v>
       </c>
@@ -2286,7 +2315,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2303,7 +2332,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="2">
         <v>17</v>
       </c>
@@ -2320,7 +2349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="2">
         <v>17</v>
       </c>
@@ -2337,7 +2366,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="8" customFormat="1">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2354,7 +2383,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="8" customFormat="1">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2371,7 +2400,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="8" customFormat="1">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2388,7 +2417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="8" customFormat="1">
       <c r="A56" s="7" t="s">
         <v>72</v>
       </c>
@@ -2405,7 +2434,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="8" customFormat="1">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2422,7 +2451,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="8" customFormat="1">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2439,7 +2468,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="8" customFormat="1">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2456,7 +2485,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="8" customFormat="1">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2473,7 +2502,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="B61" s="2">
         <v>45</v>
       </c>
@@ -2487,7 +2516,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="B62" s="2">
         <v>46</v>
       </c>
@@ -2501,7 +2530,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="B63" s="2">
         <v>47</v>
       </c>
@@ -2515,7 +2544,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="B64" s="2">
         <v>48</v>
       </c>
@@ -2529,7 +2558,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" s="8" customFormat="1">
       <c r="A65" s="7" t="s">
         <v>67</v>
       </c>
@@ -2546,7 +2575,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" s="8" customFormat="1">
       <c r="A66" s="7" t="s">
         <v>68</v>
       </c>
@@ -2563,7 +2592,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" s="8" customFormat="1">
       <c r="A67" s="7" t="s">
         <v>69</v>
       </c>
@@ -2580,7 +2609,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" s="8" customFormat="1">
       <c r="A68" s="7" t="s">
         <v>73</v>
       </c>
@@ -2597,7 +2626,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" s="8" customFormat="1">
       <c r="A69" s="7" t="s">
         <v>67</v>
       </c>
@@ -2614,7 +2643,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
         <v>67</v>
       </c>
@@ -2631,7 +2660,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" s="4" customFormat="1">
       <c r="A71" s="3" t="s">
         <v>67</v>
       </c>
@@ -2648,7 +2677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" s="4" customFormat="1">
       <c r="A72" s="3" t="s">
         <v>67</v>
       </c>
@@ -2665,7 +2694,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" s="4" customFormat="1">
       <c r="A73" s="3" t="s">
         <v>67</v>
       </c>
@@ -2682,7 +2711,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" s="4" customFormat="1">
       <c r="A74" s="3" t="s">
         <v>67</v>
       </c>
@@ -2699,7 +2728,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" s="4" customFormat="1">
       <c r="A75" s="3" t="s">
         <v>67</v>
       </c>
@@ -2716,7 +2745,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" s="4" customFormat="1">
       <c r="A76" s="3" t="s">
         <v>67</v>
       </c>
@@ -2733,7 +2762,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" s="8" customFormat="1">
       <c r="A77" s="7" t="s">
         <v>69</v>
       </c>
@@ -2750,7 +2779,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
         <v>69</v>
       </c>
@@ -2767,7 +2796,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
         <v>106</v>
       </c>
@@ -2784,7 +2813,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
         <v>106</v>
       </c>
@@ -2801,7 +2830,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
         <v>106</v>
       </c>
@@ -2818,7 +2847,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>106</v>
       </c>
@@ -2835,7 +2864,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>106</v>
       </c>
@@ -2852,7 +2881,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>106</v>
       </c>
@@ -2869,7 +2898,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" s="6" customFormat="1">
       <c r="A85" s="12" t="s">
         <v>117</v>
       </c>
@@ -2886,7 +2915,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" s="6" customFormat="1">
       <c r="A86" s="12" t="s">
         <v>121</v>
       </c>
@@ -2903,7 +2932,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" s="8" customFormat="1">
       <c r="A87" s="7" t="s">
         <v>123</v>
       </c>
@@ -2920,7 +2949,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" s="8" customFormat="1">
       <c r="A88" s="7" t="s">
         <v>123</v>
       </c>
@@ -2937,7 +2966,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" s="4" customFormat="1">
       <c r="A89" s="3" t="s">
         <v>123</v>
       </c>
@@ -2954,7 +2983,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" s="4" customFormat="1">
       <c r="A90" s="3" t="s">
         <v>131</v>
       </c>
@@ -2971,7 +3000,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" s="4" customFormat="1">
       <c r="A91" s="3" t="s">
         <v>131</v>
       </c>
@@ -2988,7 +3017,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" s="4" customFormat="1">
       <c r="A92" s="3" t="s">
         <v>131</v>
       </c>
@@ -3005,7 +3034,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" s="4" customFormat="1">
       <c r="A93" s="3" t="s">
         <v>131</v>
       </c>
@@ -3022,7 +3051,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" s="4" customFormat="1">
       <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
@@ -3039,7 +3068,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="4" customFormat="1">
       <c r="A95" s="3" t="s">
         <v>131</v>
       </c>
@@ -3056,7 +3085,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" s="4" customFormat="1">
       <c r="A96" s="3" t="s">
         <v>131</v>
       </c>
@@ -3073,7 +3102,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" s="4" customFormat="1">
       <c r="A97" s="3" t="s">
         <v>131</v>
       </c>
@@ -3090,7 +3119,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" s="4" customFormat="1">
       <c r="A98" s="3" t="s">
         <v>131</v>
       </c>
@@ -3107,7 +3136,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" s="4" customFormat="1">
       <c r="A99" s="3" t="s">
         <v>131</v>
       </c>
@@ -3124,7 +3153,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" s="4" customFormat="1">
       <c r="A100" s="3" t="s">
         <v>132</v>
       </c>
@@ -3141,7 +3170,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" s="4" customFormat="1">
       <c r="A101" s="3" t="s">
         <v>132</v>
       </c>
@@ -3158,7 +3187,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" s="4" customFormat="1">
       <c r="A102" s="3" t="s">
         <v>132</v>
       </c>
@@ -3175,7 +3204,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="4" customFormat="1">
       <c r="A103" s="3" t="s">
         <v>132</v>
       </c>
@@ -3192,7 +3221,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" s="4" customFormat="1">
       <c r="A104" s="3" t="s">
         <v>132</v>
       </c>
@@ -3209,7 +3238,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" s="4" customFormat="1">
       <c r="A105" s="3" t="s">
         <v>132</v>
       </c>
@@ -3226,7 +3255,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" s="4" customFormat="1">
       <c r="A106" s="3" t="s">
         <v>132</v>
       </c>
@@ -3243,7 +3272,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" s="4" customFormat="1">
       <c r="A107" s="3" t="s">
         <v>132</v>
       </c>
@@ -3260,7 +3289,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" s="4" customFormat="1">
       <c r="A108" s="3" t="s">
         <v>176</v>
       </c>
@@ -3277,7 +3306,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" s="4" customFormat="1">
       <c r="A109" s="3" t="s">
         <v>176</v>
       </c>
@@ -3294,7 +3323,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" s="4" customFormat="1">
       <c r="A110" s="3" t="s">
         <v>182</v>
       </c>
@@ -3311,7 +3340,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" s="4" customFormat="1">
       <c r="A111" s="3" t="s">
         <v>183</v>
       </c>
@@ -3328,7 +3357,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" s="4" customFormat="1">
       <c r="A112" s="3" t="s">
         <v>176</v>
       </c>
@@ -3345,7 +3374,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="3" t="s">
         <v>117</v>
       </c>
@@ -3362,7 +3391,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="3" t="s">
         <v>176</v>
       </c>
@@ -3379,7 +3408,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
         <v>191</v>
       </c>
@@ -3396,7 +3425,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="3" t="s">
         <v>202</v>
       </c>
@@ -3413,7 +3442,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="3" t="s">
         <v>123</v>
       </c>
@@ -3430,7 +3459,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="3" t="s">
         <v>123</v>
       </c>
@@ -3447,7 +3476,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" s="8" customFormat="1">
       <c r="A119" s="7" t="s">
         <v>183</v>
       </c>
@@ -3464,7 +3493,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" s="8" customFormat="1">
       <c r="A120" s="7" t="s">
         <v>183</v>
       </c>
@@ -3481,7 +3510,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="3" t="s">
         <v>183</v>
       </c>
@@ -3498,7 +3527,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="3" t="s">
         <v>183</v>
       </c>
@@ -3515,7 +3544,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="3" t="s">
         <v>73</v>
       </c>
@@ -3532,401 +3561,443 @@
         <v>226</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+    <row r="124" spans="1:5" s="27" customFormat="1">
+      <c r="A124" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C124" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D124" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="E124" s="3" t="s">
+      <c r="E124" s="26" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="2" t="s">
+    <row r="125" spans="1:5" s="29" customFormat="1">
+      <c r="A125" s="28"/>
+      <c r="B125" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E125" t="s">
+      <c r="D125" s="28"/>
+      <c r="E125" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C126" t="s">
+    </row>
+    <row r="127" spans="1:5" s="4" customFormat="1">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C127" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D127" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E126" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="2" t="s">
+      <c r="E127" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C127" t="s">
+    </row>
+    <row r="128" spans="1:5" s="4" customFormat="1">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C128" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D128" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E127" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="2" t="s">
+      <c r="E128" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C128" t="s">
+    </row>
+    <row r="129" spans="1:5" s="4" customFormat="1">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C129" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E128" t="s">
+      <c r="D129" s="3"/>
+      <c r="E129" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="4" customFormat="1">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="E130" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="4" customFormat="1">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C131" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E129" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B130" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="D131" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="4" customFormat="1">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C132" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E130" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="D132" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="8" customFormat="1">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C133" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E131" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C132" t="s">
+      <c r="D133" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="4" customFormat="1">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D132" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E132" t="s">
+      <c r="D134" s="3" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C133" t="s">
+      <c r="E134" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" s="4" customFormat="1">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C135" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E133" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C134" t="s">
+      <c r="D135" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="4" customFormat="1">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C136" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E134" t="s">
+      <c r="D136" s="3" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C135" t="s">
-        <v>15</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E135" t="s">
+      <c r="E136" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="2" t="s">
+    <row r="137" spans="1:5">
+      <c r="B137" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C136" t="s">
-        <v>15</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E136" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="C137" t="s">
         <v>15</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E137" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="B138" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C138" t="s">
         <v>15</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E138" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="B139" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C139" t="s">
         <v>15</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E139" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="B140" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C140" t="s">
         <v>15</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E140" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="B141" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C141" t="s">
         <v>15</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E141" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
       <c r="B142" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C142" t="s">
         <v>15</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E142" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="B143" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="E142" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="C143" t="s">
         <v>15</v>
       </c>
       <c r="D143" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E143" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="B144" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="E143" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="C144" t="s">
         <v>15</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E144" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5">
       <c r="B145" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E145" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5">
       <c r="B146" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C146" t="s">
         <v>15</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E146" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5">
       <c r="B147" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C147" t="s">
         <v>15</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E147" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5">
       <c r="B148" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C148" t="s">
         <v>15</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E148" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5">
       <c r="B149" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C149" t="s">
         <v>15</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E149" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5">
       <c r="B150" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C150" t="s">
         <v>15</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E150" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5">
       <c r="B151" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C151" t="s">
         <v>15</v>
       </c>
       <c r="E151" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5">
       <c r="B152" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C152" t="s">
         <v>15</v>
       </c>
       <c r="E152" t="s">
-        <v>289</v>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5">
+      <c r="B153" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C153" t="s">
+        <v>15</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5">
+      <c r="B154" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C154" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3936,24 +4007,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated functional reqs for movie/person pages
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\Projects\MovieDbCode\MovieDb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="341">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -91,12 +96,6 @@
   </si>
   <si>
     <t>Receive a notification when a user comments on a review.</t>
-  </si>
-  <si>
-    <t>View and Controller for displaying associated person info, i.e. What roles they've had in movies, and other biographic information. Links for admin to Edit or Delete person.</t>
-  </si>
-  <si>
-    <t>View and Controller for displaying associated movie info. Reviews and comments are displayed on the page below the movie info. Links for admin to Edit or Delete movie.</t>
   </si>
   <si>
     <t>Controller that properly deletes a person, and all corresponding person information from the database.</t>
@@ -1264,12 +1263,123 @@
   <si>
     <t>The user information section contains buttons for deleting and editing a review when the user is logged in.</t>
   </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>There are two buttons, "edit movie" and "delete movie" that only appear when an admin is logged in.</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>Movie page view/controller displays the correct information on the movie blade: title, year, release date, director, runtime, parental rating, synopsis, genre, country, and movie poster.</t>
+  </si>
+  <si>
+    <t>Person page view/controller displays the correct information on the person blade: First name, middle name, last name, first alias, middle alias, last alias,  country of origin, date of birth, date of death, biography and picture.</t>
+  </si>
+  <si>
+    <t>The pictures section of a movie page contains a partial view of the album associated with the movie. The max amount of images is 8.</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>The cast section of a movie page displays a table containing each cast member's full name, their pictures, and their role in the movie.</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>The crew section of a movie page displays a table containing each crew member's full name, their pictures, and their role in the crew.</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>The reviews sections of a movie page displays a partial view of reviews related to the movie.</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>There are two buttons, "edit person" and "delete person" that only appear when an admin is logged in.</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>There is an admin button "delete movie" that redirects to the admin's delete movie page.</t>
+  </si>
+  <si>
+    <t>There is an admin button "edit movie" that redirects to the admin's edit movie page.</t>
+  </si>
+  <si>
+    <t>There is an admin button "delete person" that redirects to the admin's delete person page.</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>There is an admin button "edit person" that redirects to the admin's edit person page.</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>The pictures section of a person page contains a partial view of the album associated with the person. The max amount of images is 8.</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>The filmography section of a person page displays a table containing each movie the person is associated with, their role in the movie, and the movie poster for the movie.</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>The discussions section of a movie page displays a partial view of discussions related to the movie.</t>
+  </si>
+  <si>
+    <t>The discussions section of a person page displays a partial view of discussions associated with that person.</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>The pictures section of a person page contains a button "view all pictures" that redirects a person to an album preview page.</t>
+  </si>
+  <si>
+    <t>The pictures section of a movie page contains a button "view all pictures" that redirects a person to an album preview page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1496,7 +1606,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1528,9 +1638,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1562,6 +1673,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1737,14 +1849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1753,40 +1865,40 @@
     <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="E2" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="E3" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" s="15" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1801,9 +1913,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -1818,9 +1930,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1829,15 +1941,15 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="4" customFormat="1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -1846,13 +1958,13 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -1866,7 +1978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -1880,7 +1992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -1894,7 +2006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -1908,7 +2020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>8</v>
       </c>
@@ -1919,10 +2031,10 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -1933,10 +2045,10 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -1950,7 +2062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -1964,7 +2076,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -1978,7 +2090,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -1992,7 +2104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -2006,7 +2118,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -2020,9 +2132,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1">
+    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B31" s="20">
         <v>16</v>
@@ -2034,12 +2146,12 @@
         <v>6</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="24" customFormat="1">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B32" s="23">
         <v>17</v>
@@ -2051,12 +2163,12 @@
         <v>6</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="24" customFormat="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B33" s="23">
         <v>18</v>
@@ -2068,15 +2180,15 @@
         <v>6</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="24" customFormat="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>16</v>
@@ -2085,12 +2197,12 @@
         <v>6</v>
       </c>
       <c r="E34" s="25" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="24" customFormat="1">
-      <c r="A35" s="22" t="s">
-        <v>299</v>
       </c>
       <c r="B35" s="23">
         <v>19</v>
@@ -2099,15 +2211,15 @@
         <v>16</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="24" customFormat="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B36" s="23">
         <v>20</v>
@@ -2116,15 +2228,15 @@
         <v>16</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="14" customFormat="1">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B37" s="16">
         <v>21</v>
@@ -2133,15 +2245,15 @@
         <v>16</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="14" customFormat="1">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B38" s="16">
         <v>22</v>
@@ -2150,16 +2262,16 @@
         <v>16</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="9" customFormat="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>4</v>
@@ -2168,13 +2280,13 @@
         <v>6</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="9" customFormat="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>4</v>
@@ -2183,38 +2295,38 @@
         <v>6</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D41" s="2">
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2222,13 +2334,13 @@
         <v>13</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" t="s">
         <v>33</v>
       </c>
-      <c r="E43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2236,69 +2348,69 @@
         <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" t="s">
         <v>34</v>
       </c>
-      <c r="E44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>30</v>
       </c>
       <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D48" s="2">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>16</v>
       </c>
@@ -2306,16 +2418,16 @@
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2329,10 +2441,10 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>17</v>
       </c>
@@ -2346,10 +2458,10 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>17</v>
       </c>
@@ -2363,10 +2475,10 @@
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="8" customFormat="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2374,16 +2486,16 @@
         <v>37</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="8" customFormat="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2391,16 +2503,16 @@
         <v>38</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="8" customFormat="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2408,33 +2520,33 @@
         <v>39</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="8" customFormat="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B56" s="7">
         <v>40</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="8" customFormat="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2442,16 +2554,16 @@
         <v>41</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D57" s="7">
         <v>40</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="8" customFormat="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2459,16 +2571,16 @@
         <v>42</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="8" customFormat="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2476,16 +2588,16 @@
         <v>43</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="8" customFormat="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2493,842 +2605,842 @@
         <v>44</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="8" customFormat="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" s="7">
         <v>49</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="8" customFormat="1">
-      <c r="A66" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="B66" s="7">
         <v>50</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="8" customFormat="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B67" s="7">
         <v>51</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E67" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" s="8" customFormat="1">
-      <c r="A68" s="7" t="s">
+      <c r="B68" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="E68" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D68" s="7" t="s">
+    </row>
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="C69" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" s="8" customFormat="1">
-      <c r="A69" s="7" t="s">
+      <c r="E69" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E69" s="7" t="s">
+      <c r="B77" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C70" t="s">
-        <v>65</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="4" customFormat="1">
-      <c r="A71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="4" customFormat="1">
-      <c r="A72" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="4" customFormat="1">
-      <c r="A73" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="4" customFormat="1">
-      <c r="A74" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="4" customFormat="1">
-      <c r="A75" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="4" customFormat="1">
-      <c r="A76" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="3" t="s">
+      <c r="C78" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" s="8" customFormat="1">
-      <c r="A77" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E77" s="7" t="s">
+      <c r="D78" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B78" s="3" t="s">
+      <c r="E78" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D78" s="3" t="s">
+      <c r="C79" t="s">
+        <v>58</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B79" s="2" t="s">
+      <c r="C80" t="s">
+        <v>58</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C79" t="s">
-        <v>60</v>
-      </c>
-      <c r="D79" s="2" t="s">
+      <c r="C81" t="s">
+        <v>58</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C82" t="s">
+        <v>58</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B80" s="2" t="s">
+      <c r="E82" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C83" t="s">
+        <v>58</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C80" t="s">
-        <v>60</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B81" s="2" t="s">
+      <c r="E83" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C81" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="2" t="s">
+      <c r="B84" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C84" t="s">
+        <v>58</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C83" t="s">
-        <v>60</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E83" s="2" t="s">
+      <c r="E84" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C84" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E84" s="2" t="s">
+      <c r="B85" s="12" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" s="6" customFormat="1">
-      <c r="A85" s="12" t="s">
+      <c r="C85" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="12" t="s">
+    </row>
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B86" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C85" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="6" customFormat="1">
-      <c r="A86" s="12" t="s">
+      <c r="C86" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E86" s="12" t="s">
+      <c r="B87" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" s="8" customFormat="1">
-      <c r="A87" s="7" t="s">
+      <c r="C87" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="C88" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="8" customFormat="1">
-      <c r="A88" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E88" s="7" t="s">
+    </row>
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" s="4" customFormat="1">
-      <c r="A89" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="4" customFormat="1">
-      <c r="A90" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="4" customFormat="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="4" customFormat="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="4" customFormat="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="4" customFormat="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" s="4" customFormat="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="4" customFormat="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" s="4" customFormat="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" s="4" customFormat="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="4" customFormat="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" s="4" customFormat="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="4" customFormat="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" s="4" customFormat="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" s="4" customFormat="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="4" customFormat="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" s="4" customFormat="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="4" customFormat="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" s="4" customFormat="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" s="4" customFormat="1">
-      <c r="A108" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" s="4" customFormat="1">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="4" customFormat="1">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>4</v>
@@ -3337,15 +3449,15 @@
         <v>6</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" s="4" customFormat="1">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>4</v>
@@ -3354,134 +3466,134 @@
         <v>6</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" s="4" customFormat="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E112" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
-      <c r="A113" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B113" s="3" t="s">
+      <c r="C113" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E113" s="3" t="s">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
-      <c r="A114" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E114" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="C115" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D116" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D116" s="3" t="s">
+      <c r="E116" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E116" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
-      <c r="A117" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B117" s="3" t="s">
+      <c r="D117" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D117" s="3" t="s">
+    </row>
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="C118" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
-      <c r="A118" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B118" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C118" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D118" s="3" t="s">
+    </row>
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B119" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" s="8" customFormat="1">
-      <c r="A119" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>4</v>
@@ -3490,15 +3602,15 @@
         <v>6</v>
       </c>
       <c r="E119" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B120" s="7" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" s="8" customFormat="1">
-      <c r="A120" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>4</v>
@@ -3507,497 +3619,697 @@
         <v>6</v>
       </c>
       <c r="E120" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
-      <c r="A121" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E122" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B123" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
-      <c r="A123" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B123" s="3" t="s">
+      <c r="C123" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C123" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D123" s="3" t="s">
+    </row>
+    <row r="124" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B124" s="26" t="s">
         <v>225</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" s="27" customFormat="1">
-      <c r="A124" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B124" s="26" t="s">
-        <v>227</v>
       </c>
       <c r="C124" s="27" t="s">
         <v>4</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" s="29" customFormat="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="28"/>
       <c r="B125" s="28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C125" s="29" t="s">
         <v>15</v>
       </c>
       <c r="D125" s="28"/>
       <c r="E125" s="29" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E126" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
+    </row>
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" s="4" customFormat="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" s="4" customFormat="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" s="8" customFormat="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" s="4" customFormat="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" s="4" customFormat="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" s="4" customFormat="1">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D136" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E136" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E136" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B137" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C137" t="s">
         <v>15</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E137" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B138" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C138" t="s">
         <v>15</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E138" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B139" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C139" t="s">
         <v>15</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E139" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C140" t="s">
         <v>15</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E140" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B141" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C141" t="s">
         <v>15</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E141" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C142" t="s">
         <v>15</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E142" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B143" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="E142" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="B143" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="C143" t="s">
         <v>15</v>
       </c>
       <c r="D143" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E143" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B144" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="E143" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="B144" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="C144" t="s">
         <v>15</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E144" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B145" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C145" t="s">
         <v>15</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E145" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C146" t="s">
         <v>15</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E146" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C147" t="s">
         <v>15</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E147" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C148" t="s">
         <v>15</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E148" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C149" t="s">
         <v>15</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E149" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B150" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C150" t="s">
         <v>15</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E150" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C151" t="s">
         <v>15</v>
       </c>
       <c r="E151" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C152" t="s">
         <v>15</v>
       </c>
       <c r="E152" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C153" t="s">
         <v>15</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C154" t="s">
         <v>15</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C155" t="s">
+        <v>305</v>
+      </c>
+      <c r="E155" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B156" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C156" t="s">
+        <v>305</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E156" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C157" t="s">
+        <v>305</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E157" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C158" t="s">
+        <v>305</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E158" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C159" t="s">
+        <v>305</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E159" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C160" t="s">
+        <v>305</v>
+      </c>
+      <c r="E160" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B161" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C161" t="s">
+        <v>305</v>
+      </c>
+      <c r="E161" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C162" t="s">
+        <v>305</v>
+      </c>
+      <c r="E162" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B163" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C163" t="s">
+        <v>305</v>
+      </c>
+      <c r="E163" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B164" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C164" t="s">
+        <v>199</v>
+      </c>
+      <c r="E164" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B165" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C165" t="s">
+        <v>199</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E165" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B166" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C166" t="s">
+        <v>199</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E166" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B167" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C167" t="s">
+        <v>199</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E167" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B168" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C168" t="s">
+        <v>199</v>
+      </c>
+      <c r="E168" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B169" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C169" t="s">
+        <v>199</v>
+      </c>
+      <c r="E169" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B170" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C170" t="s">
+        <v>199</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4007,24 +4319,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Review Testing reflected in functional_reqs.
Review Testing reflected in functional_reqs.
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\Projects\MovieDbCode\MovieDb\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -1207,9 +1202,6 @@
     <t>136</t>
   </si>
   <si>
-    <t>If a user attempts to display a review that does no exist, a review not found page is displayed.</t>
-  </si>
-  <si>
     <t>TESTING IN PROGRESS</t>
   </si>
   <si>
@@ -1373,13 +1365,16 @@
   </si>
   <si>
     <t>The pictures section of a movie page contains a button "view all pictures" that redirects a person to an album preview page.</t>
+  </si>
+  <si>
+    <t>If a user attempts to display a review that does not exist, a review not found page is displayed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1606,7 +1601,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1638,10 +1633,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1673,7 +1667,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1849,14 +1842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125:XFD125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1865,38 +1858,38 @@
     <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="E2" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="E3" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="E4" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="E5" s="9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="E6" s="15" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1913,7 +1906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="8" customFormat="1">
       <c r="A16" s="7" t="s">
         <v>128</v>
       </c>
@@ -1930,7 +1923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="4" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>129</v>
       </c>
@@ -1947,7 +1940,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="4" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>130</v>
       </c>
@@ -1964,7 +1957,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -1978,7 +1971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -1992,7 +1985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -2006,7 +1999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -2020,7 +2013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="B23" s="2">
         <v>8</v>
       </c>
@@ -2031,10 +2024,10 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -2045,10 +2038,10 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -2062,7 +2055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -2076,7 +2069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -2090,7 +2083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -2104,7 +2097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -2118,7 +2111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -2132,9 +2125,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="21" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B31" s="20">
         <v>16</v>
@@ -2146,12 +2139,12 @@
         <v>6</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="24" customFormat="1">
       <c r="A32" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B32" s="23">
         <v>17</v>
@@ -2163,12 +2156,12 @@
         <v>6</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="24" customFormat="1">
       <c r="A33" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B33" s="23">
         <v>18</v>
@@ -2180,15 +2173,15 @@
         <v>6</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="24" customFormat="1">
       <c r="A34" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C34" s="25" t="s">
         <v>16</v>
@@ -2197,12 +2190,12 @@
         <v>6</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="24" customFormat="1">
       <c r="A35" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B35" s="23">
         <v>19</v>
@@ -2211,15 +2204,15 @@
         <v>16</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="24" customFormat="1">
       <c r="A36" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B36" s="23">
         <v>20</v>
@@ -2228,15 +2221,15 @@
         <v>16</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1">
       <c r="A37" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B37" s="16">
         <v>21</v>
@@ -2248,12 +2241,12 @@
         <v>104</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="14" customFormat="1">
       <c r="A38" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B38" s="16">
         <v>22</v>
@@ -2268,7 +2261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="9" customFormat="1">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>202</v>
@@ -2283,7 +2276,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="9" customFormat="1">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>115</v>
@@ -2298,7 +2291,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="B41" s="2">
         <v>25</v>
       </c>
@@ -2312,7 +2305,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="B42" s="2">
         <v>26</v>
       </c>
@@ -2326,7 +2319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2340,7 +2333,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2354,7 +2347,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="B45" s="2">
         <v>29</v>
       </c>
@@ -2368,7 +2361,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="B46" s="2">
         <v>30</v>
       </c>
@@ -2382,7 +2375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="B47" s="2">
         <v>31</v>
       </c>
@@ -2396,7 +2389,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="B48" s="2">
         <v>32</v>
       </c>
@@ -2410,7 +2403,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="2">
         <v>16</v>
       </c>
@@ -2427,7 +2420,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2444,7 +2437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="2">
         <v>17</v>
       </c>
@@ -2461,7 +2454,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="2">
         <v>17</v>
       </c>
@@ -2478,7 +2471,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="8" customFormat="1">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2495,7 +2488,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="8" customFormat="1">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2512,7 +2505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="8" customFormat="1">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2529,7 +2522,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="8" customFormat="1">
       <c r="A56" s="7" t="s">
         <v>70</v>
       </c>
@@ -2546,7 +2539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="8" customFormat="1">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2563,7 +2556,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="8" customFormat="1">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2580,7 +2573,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="8" customFormat="1">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2597,7 +2590,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="8" customFormat="1">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2614,7 +2607,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="B61" s="2">
         <v>45</v>
       </c>
@@ -2628,7 +2621,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="B62" s="2">
         <v>46</v>
       </c>
@@ -2642,7 +2635,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="B63" s="2">
         <v>47</v>
       </c>
@@ -2656,7 +2649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="B64" s="2">
         <v>48</v>
       </c>
@@ -2670,7 +2663,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" s="8" customFormat="1">
       <c r="A65" s="7" t="s">
         <v>65</v>
       </c>
@@ -2687,7 +2680,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" s="8" customFormat="1">
       <c r="A66" s="7" t="s">
         <v>66</v>
       </c>
@@ -2704,7 +2697,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" s="8" customFormat="1">
       <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
@@ -2721,7 +2714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" s="8" customFormat="1">
       <c r="A68" s="7" t="s">
         <v>71</v>
       </c>
@@ -2738,7 +2731,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" s="8" customFormat="1">
       <c r="A69" s="7" t="s">
         <v>65</v>
       </c>
@@ -2755,7 +2748,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
         <v>65</v>
       </c>
@@ -2772,7 +2765,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" s="4" customFormat="1">
       <c r="A71" s="3" t="s">
         <v>65</v>
       </c>
@@ -2789,7 +2782,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" s="4" customFormat="1">
       <c r="A72" s="3" t="s">
         <v>65</v>
       </c>
@@ -2806,7 +2799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" s="4" customFormat="1">
       <c r="A73" s="3" t="s">
         <v>65</v>
       </c>
@@ -2823,7 +2816,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" s="4" customFormat="1">
       <c r="A74" s="3" t="s">
         <v>65</v>
       </c>
@@ -2840,7 +2833,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" s="4" customFormat="1">
       <c r="A75" s="3" t="s">
         <v>65</v>
       </c>
@@ -2857,7 +2850,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" s="4" customFormat="1">
       <c r="A76" s="3" t="s">
         <v>65</v>
       </c>
@@ -2874,7 +2867,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" s="8" customFormat="1">
       <c r="A77" s="7" t="s">
         <v>67</v>
       </c>
@@ -2891,7 +2884,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
         <v>67</v>
       </c>
@@ -2908,7 +2901,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
         <v>104</v>
       </c>
@@ -2925,7 +2918,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
@@ -2942,7 +2935,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -2959,7 +2952,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>104</v>
       </c>
@@ -2976,7 +2969,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>104</v>
       </c>
@@ -2993,7 +2986,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>104</v>
       </c>
@@ -3010,7 +3003,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" s="6" customFormat="1">
       <c r="A85" s="12" t="s">
         <v>115</v>
       </c>
@@ -3027,7 +3020,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" s="6" customFormat="1">
       <c r="A86" s="12" t="s">
         <v>119</v>
       </c>
@@ -3044,7 +3037,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" s="8" customFormat="1">
       <c r="A87" s="7" t="s">
         <v>121</v>
       </c>
@@ -3061,7 +3054,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" s="8" customFormat="1">
       <c r="A88" s="7" t="s">
         <v>121</v>
       </c>
@@ -3078,7 +3071,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" s="4" customFormat="1">
       <c r="A89" s="3" t="s">
         <v>121</v>
       </c>
@@ -3095,7 +3088,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" s="4" customFormat="1">
       <c r="A90" s="3" t="s">
         <v>129</v>
       </c>
@@ -3112,7 +3105,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" s="4" customFormat="1">
       <c r="A91" s="3" t="s">
         <v>129</v>
       </c>
@@ -3129,7 +3122,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" s="4" customFormat="1">
       <c r="A92" s="3" t="s">
         <v>129</v>
       </c>
@@ -3146,7 +3139,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" s="4" customFormat="1">
       <c r="A93" s="3" t="s">
         <v>129</v>
       </c>
@@ -3163,7 +3156,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" s="4" customFormat="1">
       <c r="A94" s="3" t="s">
         <v>129</v>
       </c>
@@ -3180,7 +3173,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="4" customFormat="1">
       <c r="A95" s="3" t="s">
         <v>129</v>
       </c>
@@ -3197,7 +3190,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" s="4" customFormat="1">
       <c r="A96" s="3" t="s">
         <v>129</v>
       </c>
@@ -3214,7 +3207,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" s="4" customFormat="1">
       <c r="A97" s="3" t="s">
         <v>129</v>
       </c>
@@ -3231,7 +3224,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" s="4" customFormat="1">
       <c r="A98" s="3" t="s">
         <v>129</v>
       </c>
@@ -3248,7 +3241,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" s="4" customFormat="1">
       <c r="A99" s="3" t="s">
         <v>129</v>
       </c>
@@ -3265,7 +3258,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" s="4" customFormat="1">
       <c r="A100" s="3" t="s">
         <v>130</v>
       </c>
@@ -3282,7 +3275,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" s="4" customFormat="1">
       <c r="A101" s="3" t="s">
         <v>130</v>
       </c>
@@ -3299,7 +3292,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" s="4" customFormat="1">
       <c r="A102" s="3" t="s">
         <v>130</v>
       </c>
@@ -3316,7 +3309,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="4" customFormat="1">
       <c r="A103" s="3" t="s">
         <v>130</v>
       </c>
@@ -3333,7 +3326,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" s="4" customFormat="1">
       <c r="A104" s="3" t="s">
         <v>130</v>
       </c>
@@ -3350,7 +3343,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" s="4" customFormat="1">
       <c r="A105" s="3" t="s">
         <v>130</v>
       </c>
@@ -3367,7 +3360,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" s="4" customFormat="1">
       <c r="A106" s="3" t="s">
         <v>130</v>
       </c>
@@ -3384,7 +3377,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" s="4" customFormat="1">
       <c r="A107" s="3" t="s">
         <v>130</v>
       </c>
@@ -3401,7 +3394,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" s="4" customFormat="1">
       <c r="A108" s="3" t="s">
         <v>174</v>
       </c>
@@ -3418,7 +3411,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" s="4" customFormat="1">
       <c r="A109" s="3" t="s">
         <v>174</v>
       </c>
@@ -3435,7 +3428,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" s="4" customFormat="1">
       <c r="A110" s="3" t="s">
         <v>180</v>
       </c>
@@ -3452,7 +3445,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" s="4" customFormat="1">
       <c r="A111" s="3" t="s">
         <v>181</v>
       </c>
@@ -3469,7 +3462,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" s="4" customFormat="1">
       <c r="A112" s="3" t="s">
         <v>174</v>
       </c>
@@ -3486,7 +3479,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="3" t="s">
         <v>115</v>
       </c>
@@ -3503,7 +3496,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" s="4" customFormat="1">
       <c r="A114" s="3" t="s">
         <v>174</v>
       </c>
@@ -3520,7 +3513,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="3" t="s">
         <v>189</v>
       </c>
@@ -3537,7 +3530,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="3" t="s">
         <v>200</v>
       </c>
@@ -3554,7 +3547,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" s="4" customFormat="1">
       <c r="A117" s="3" t="s">
         <v>121</v>
       </c>
@@ -3571,7 +3564,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" s="4" customFormat="1">
       <c r="A118" s="3" t="s">
         <v>121</v>
       </c>
@@ -3588,7 +3581,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" s="8" customFormat="1">
       <c r="A119" s="7" t="s">
         <v>181</v>
       </c>
@@ -3605,7 +3598,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" s="8" customFormat="1">
       <c r="A120" s="7" t="s">
         <v>181</v>
       </c>
@@ -3622,7 +3615,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" s="4" customFormat="1">
       <c r="A121" s="3" t="s">
         <v>181</v>
       </c>
@@ -3639,7 +3632,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" s="4" customFormat="1">
       <c r="A122" s="3" t="s">
         <v>181</v>
       </c>
@@ -3656,7 +3649,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" s="4" customFormat="1">
       <c r="A123" s="3" t="s">
         <v>71</v>
       </c>
@@ -3673,7 +3666,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" s="27" customFormat="1">
       <c r="A124" s="26" t="s">
         <v>174</v>
       </c>
@@ -3690,7 +3683,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" s="29" customFormat="1">
       <c r="A125" s="28"/>
       <c r="B125" s="28" t="s">
         <v>230</v>
@@ -3700,10 +3693,10 @@
       </c>
       <c r="D125" s="28"/>
       <c r="E125" s="29" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
         <v>231</v>
@@ -3718,7 +3711,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" s="4" customFormat="1">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>233</v>
@@ -3733,7 +3726,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" s="4" customFormat="1">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
         <v>235</v>
@@ -3748,7 +3741,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" s="4" customFormat="1">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
         <v>237</v>
@@ -3761,7 +3754,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" s="4" customFormat="1">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>239</v>
@@ -3776,7 +3769,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" s="4" customFormat="1">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
         <v>241</v>
@@ -3791,7 +3784,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" s="4" customFormat="1">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>243</v>
@@ -3806,7 +3799,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" s="8" customFormat="1">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
         <v>245</v>
@@ -3821,7 +3814,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" s="4" customFormat="1">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>247</v>
@@ -3836,7 +3829,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" s="4" customFormat="1">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>249</v>
@@ -3848,10 +3841,10 @@
         <v>245</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="4" customFormat="1">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>250</v>
@@ -3866,391 +3859,411 @@
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="2" t="s">
+    <row r="137" spans="1:5" s="4" customFormat="1">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D137" s="2" t="s">
+      <c r="D137" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="2" t="s">
+    <row r="138" spans="1:5" s="4" customFormat="1">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="D138" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B139" s="2" t="s">
+    <row r="139" spans="1:5" s="4" customFormat="1">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="D139" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="2" t="s">
+    <row r="140" spans="1:5" s="4" customFormat="1">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="D140" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B141" s="2" t="s">
+    <row r="141" spans="1:5" s="4" customFormat="1">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D141" s="2" t="s">
+      <c r="D141" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="2" t="s">
+    <row r="142" spans="1:5" s="4" customFormat="1">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="D142" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="2" t="s">
+    <row r="143" spans="1:5" s="4" customFormat="1">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D143" s="2" t="s">
+      <c r="D143" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="2" t="s">
+    <row r="144" spans="1:5" s="4" customFormat="1">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D144" s="2" t="s">
+      <c r="D144" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="2" t="s">
+    <row r="145" spans="1:5" s="4" customFormat="1">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D145" s="2" t="s">
+      <c r="D145" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146" s="2" t="s">
+    <row r="146" spans="1:5" s="4" customFormat="1">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D146" s="2" t="s">
+      <c r="D146" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E146" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="2" t="s">
+    <row r="147" spans="1:5" s="4" customFormat="1">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D147" s="2" t="s">
+      <c r="D147" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="2" t="s">
+    <row r="148" spans="1:5" s="4" customFormat="1">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D148" s="2" t="s">
+      <c r="D148" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="2" t="s">
+    <row r="149" spans="1:5" s="4" customFormat="1">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D149" s="2" t="s">
+      <c r="D149" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="2" t="s">
+    <row r="150" spans="1:5" s="4" customFormat="1">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D150" s="2" t="s">
+      <c r="D150" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B151" s="2" t="s">
+    <row r="151" spans="1:5" s="4" customFormat="1">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E151" t="s">
+      <c r="D151" s="3"/>
+      <c r="E151" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="2" t="s">
+    <row r="152" spans="1:5" s="4" customFormat="1">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E152" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B153" s="2" t="s">
+      <c r="D152" s="3"/>
+      <c r="E152" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" s="4" customFormat="1">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E153" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="C153" t="s">
+    </row>
+    <row r="154" spans="1:5" s="4" customFormat="1">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C154" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D153" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="2" t="s">
+      <c r="D154" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E154" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C154" t="s">
-        <v>15</v>
-      </c>
-      <c r="D154" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E154" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:5">
       <c r="B155" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C155" t="s">
         <v>304</v>
       </c>
-      <c r="C155" t="s">
+      <c r="E155" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="B156" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="E155" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="2" t="s">
+      <c r="C156" t="s">
+        <v>304</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E156" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="B157" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C156" t="s">
-        <v>305</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="E156" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="C157" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>104</v>
       </c>
       <c r="E157" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
       <c r="B158" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C158" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E158" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="B159" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="C159" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E159" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
       <c r="B160" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C160" t="s">
+        <v>304</v>
+      </c>
+      <c r="E160" t="s">
         <v>314</v>
       </c>
-      <c r="C160" t="s">
-        <v>305</v>
-      </c>
-      <c r="E160" t="s">
+    </row>
+    <row r="161" spans="2:5">
+      <c r="B161" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="2" t="s">
+      <c r="C161" t="s">
+        <v>304</v>
+      </c>
+      <c r="E161" t="s">
         <v>316</v>
       </c>
-      <c r="C161" t="s">
-        <v>305</v>
-      </c>
-      <c r="E161" t="s">
+    </row>
+    <row r="162" spans="2:5">
+      <c r="B162" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B162" s="2" t="s">
+      <c r="C162" t="s">
+        <v>304</v>
+      </c>
+      <c r="E162" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5">
+      <c r="B163" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C162" t="s">
-        <v>305</v>
-      </c>
-      <c r="E162" t="s">
+      <c r="C163" t="s">
+        <v>304</v>
+      </c>
+      <c r="E163" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5">
+      <c r="B164" s="2" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B163" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C163" t="s">
-        <v>305</v>
-      </c>
-      <c r="E163" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B164" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C164" t="s">
         <v>199</v>
       </c>
       <c r="E164" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5">
+      <c r="B165" s="2" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="C165" t="s">
         <v>199</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E165" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5">
+      <c r="B166" s="2" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="C166" t="s">
         <v>199</v>
@@ -4259,12 +4272,12 @@
         <v>71</v>
       </c>
       <c r="E166" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5">
+      <c r="B167" s="2" t="s">
         <v>328</v>
-      </c>
-    </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="C167" t="s">
         <v>199</v>
@@ -4273,34 +4286,34 @@
         <v>116</v>
       </c>
       <c r="E167" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5">
+      <c r="B168" s="2" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="C168" t="s">
         <v>199</v>
       </c>
       <c r="E168" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5">
+      <c r="B169" s="2" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B169" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="C169" t="s">
         <v>199</v>
       </c>
       <c r="E169" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5">
       <c r="B170" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C170" t="s">
         <v>199</v>
@@ -4309,7 +4322,7 @@
         <v>122</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -4319,24 +4332,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated functional requirements; testing documentation
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MovieDbCode\MovieDb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
   </bookViews>
@@ -1373,8 +1378,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1419,7 +1424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1467,6 +1472,12 @@
         <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1497,11 +1508,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1530,6 +1538,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1540,9 +1553,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9966"/>
       <color rgb="FF99FF99"/>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFF99FF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF6666FF"/>
     </mruColors>
@@ -1601,7 +1615,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1633,9 +1647,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1667,6 +1682,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1842,1073 +1858,1079 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125:XFD125"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="C1" s="5"/>
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="4"/>
+      <c r="E1" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="E2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="E3" s="7" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="6" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="E5" s="9" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="8" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="E6" s="15" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="14" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>3</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="B19" s="2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
         <v>4</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="B20" s="2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
         <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="B21" s="2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="B22" s="2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
         <v>8</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="B24" s="2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>9</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="B25" s="2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="B26" s="2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
         <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>8</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
         <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>11</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="B28" s="2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
         <v>13</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>11</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="B29" s="2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
         <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>11</v>
       </c>
       <c r="E29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
         <v>15</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>13</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1">
-      <c r="A31" s="19" t="s">
+    <row r="31" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="19">
         <v>16</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="20" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="24" customFormat="1">
-      <c r="A32" s="22" t="s">
+    <row r="32" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <v>17</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="24" customFormat="1">
-      <c r="A33" s="22" t="s">
+    <row r="33" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <v>18</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="24" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="24" customFormat="1">
-      <c r="A34" s="22" t="s">
+    <row r="34" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="24" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="24" customFormat="1">
-      <c r="A35" s="22" t="s">
+    <row r="35" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>19</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="24" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="24" customFormat="1">
-      <c r="A36" s="22" t="s">
+    <row r="36" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="22">
         <v>20</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="24" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="14" customFormat="1">
-      <c r="A37" s="17" t="s">
+    <row r="37" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="15">
         <v>21</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="14" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="14" customFormat="1">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="15">
         <v>22</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10" t="s">
+    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10" t="s">
+    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="B41" s="2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9">
         <v>25</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="9">
         <v>6</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
       <c r="B42" s="2">
         <v>26</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="B43" s="2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
         <v>27</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="B44" s="2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
         <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="B45" s="2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
         <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="B46" s="2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
         <v>30</v>
       </c>
       <c r="C46" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="B47" s="2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
         <v>31</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="B48" s="2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
         <v>32</v>
       </c>
       <c r="C48" t="s">
         <v>35</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>6</v>
       </c>
       <c r="E48" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>16</v>
       </c>
-      <c r="B49" s="18">
+      <c r="B49" s="17">
         <v>33</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>17</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>34</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>17</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>35</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E51" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>17</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>36</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E52" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1">
-      <c r="A53" s="7">
+    <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
         <v>6</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="6">
         <v>37</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="8" customFormat="1">
-      <c r="A54" s="7">
+    <row r="54" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
         <v>3</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <v>38</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="8" customFormat="1">
-      <c r="A55" s="7">
+    <row r="55" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
         <v>5</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="6">
         <v>39</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1">
-      <c r="A56" s="7" t="s">
+    <row r="56" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <v>40</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="8" customFormat="1">
-      <c r="A57" s="7">
+    <row r="57" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
         <v>10</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <v>41</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="6">
         <v>40</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="8" customFormat="1">
-      <c r="A58" s="7">
+    <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
         <v>18</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="6">
         <v>42</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="8" customFormat="1">
-      <c r="A59" s="7">
+    <row r="59" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
         <v>6</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="6">
         <v>43</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="8" customFormat="1">
-      <c r="A60" s="7">
+    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
         <v>6</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <v>44</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="B61" s="2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="30"/>
+      <c r="B61" s="30">
         <v>45</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
-      <c r="B62" s="2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="30"/>
+      <c r="B62" s="30">
         <v>46</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="B63" s="2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="30"/>
+      <c r="B63" s="30">
         <v>47</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
-      <c r="B64" s="2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="30"/>
+      <c r="B64" s="30">
         <v>48</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="8" customFormat="1">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="6">
         <v>49</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E65" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="8" customFormat="1">
-      <c r="A66" s="7" t="s">
+    <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="6">
         <v>50</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="8" customFormat="1">
-      <c r="A67" s="7" t="s">
+    <row r="67" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="6">
         <v>51</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E67" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="8" customFormat="1">
-      <c r="A68" s="7" t="s">
+    <row r="68" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="8" customFormat="1">
-      <c r="A69" s="7" t="s">
+    <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="2" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C70" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="E74" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E76" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="8" customFormat="1">
-      <c r="A77" s="7" t="s">
+    <row r="77" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="E77" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -2918,14 +2940,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -2935,48 +2957,48 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="2" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E81" s="30" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="2" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E82" s="30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D83" s="2" t="s">
@@ -2986,14 +3008,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D84" s="2" t="s">
@@ -3003,1130 +3025,1130 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1">
-      <c r="A85" s="12" t="s">
+    <row r="85" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E85" s="12" t="s">
+      <c r="E85" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1">
-      <c r="A86" s="12" t="s">
+    <row r="86" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E86" s="12" t="s">
+      <c r="E86" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="8" customFormat="1">
-      <c r="A87" s="7" t="s">
+    <row r="87" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E87" s="7" t="s">
+      <c r="E87" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="8" customFormat="1">
-      <c r="A88" s="7" t="s">
+    <row r="88" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="E88" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E89" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E90" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E91" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E92" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="E94" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1">
-      <c r="A95" s="3" t="s">
+    <row r="95" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E95" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E96" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E97" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1">
-      <c r="A98" s="3" t="s">
+    <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D98" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E98" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1">
-      <c r="A99" s="3" t="s">
+    <row r="99" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E99" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E100" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1">
-      <c r="A101" s="3" t="s">
+    <row r="101" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E101" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1">
-      <c r="A102" s="3" t="s">
+    <row r="102" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E102" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1">
-      <c r="A103" s="3" t="s">
+    <row r="103" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C103" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D103" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E103" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1">
-      <c r="A104" s="3" t="s">
+    <row r="104" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D104" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E104" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="4" customFormat="1">
-      <c r="A105" s="3" t="s">
+    <row r="105" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C105" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="D105" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E105" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1">
-      <c r="A107" s="3" t="s">
+    <row r="107" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="E107" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1">
-      <c r="A108" s="3" t="s">
+    <row r="108" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E108" s="3" t="s">
+      <c r="E108" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1">
-      <c r="A109" s="3" t="s">
+    <row r="109" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="E109" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1">
-      <c r="A110" s="3" t="s">
+    <row r="110" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="E110" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1">
-      <c r="A111" s="3" t="s">
+    <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C111" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E111" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1">
-      <c r="A112" s="3" t="s">
+    <row r="112" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D112" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="E112" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
-      <c r="A113" s="3" t="s">
+    <row r="113" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C113" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D113" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E113" s="3" t="s">
+      <c r="E113" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D114" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="E114" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="3" t="s">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C115" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D115" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E115" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
-      <c r="A116" s="3" t="s">
+    <row r="116" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="E116" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
-      <c r="A117" s="3" t="s">
+    <row r="117" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E117" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
-      <c r="A118" s="3" t="s">
+    <row r="118" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="E118" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="8" customFormat="1">
-      <c r="A119" s="7" t="s">
+    <row r="119" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="B119" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C119" s="8" t="s">
+      <c r="C119" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="D119" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E119" s="7" t="s">
+      <c r="E119" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="8" customFormat="1">
-      <c r="A120" s="7" t="s">
+    <row r="120" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B120" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C120" s="8" t="s">
+      <c r="C120" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D120" s="7" t="s">
+      <c r="D120" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E120" s="7" t="s">
+      <c r="E120" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
-      <c r="A121" s="3" t="s">
+    <row r="121" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C121" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E121" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
-      <c r="A122" s="3" t="s">
+    <row r="122" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C122" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D122" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="E122" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
-      <c r="A123" s="3" t="s">
+    <row r="123" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C123" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="E123" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="27" customFormat="1">
-      <c r="A124" s="26" t="s">
+    <row r="124" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="B124" s="26" t="s">
+      <c r="B124" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="C124" s="27" t="s">
+      <c r="C124" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D124" s="26" t="s">
+      <c r="D124" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="E124" s="26" t="s">
+      <c r="E124" s="25" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="29" customFormat="1">
-      <c r="A125" s="28"/>
-      <c r="B125" s="28" t="s">
+    <row r="125" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="27"/>
+      <c r="B125" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="C125" s="29" t="s">
+      <c r="C125" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D125" s="28"/>
-      <c r="E125" s="29" t="s">
+      <c r="D125" s="27"/>
+      <c r="E125" s="28" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3" t="s">
+    <row r="126" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D126" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E126" s="4" t="s">
+      <c r="E126" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3" t="s">
+    <row r="127" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C127" s="4" t="s">
+      <c r="C127" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D127" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E127" s="4" t="s">
+      <c r="E127" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3" t="s">
+    <row r="128" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D128" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E128" s="4" t="s">
+      <c r="E128" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
-      <c r="A129" s="3"/>
-      <c r="B129" s="3" t="s">
+    <row r="129" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="C129" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D129" s="3"/>
-      <c r="E129" s="4" t="s">
+      <c r="D129" s="2"/>
+      <c r="E129" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
-      <c r="A130" s="3"/>
-      <c r="B130" s="3" t="s">
+    <row r="130" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+      <c r="B130" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D130" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E130" s="4" t="s">
+      <c r="E130" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="4" customFormat="1">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3" t="s">
+    <row r="131" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+      <c r="B131" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D131" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E131" s="4" t="s">
+      <c r="E131" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3" t="s">
+    <row r="132" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C132" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D132" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E132" s="4" t="s">
+      <c r="E132" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="8" customFormat="1">
-      <c r="A133" s="7"/>
-      <c r="B133" s="7" t="s">
+    <row r="133" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="6"/>
+      <c r="B133" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C133" s="8" t="s">
+      <c r="C133" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D133" s="7" t="s">
+      <c r="D133" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E133" s="8" t="s">
+      <c r="E133" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1">
-      <c r="A134" s="3"/>
-      <c r="B134" s="3" t="s">
+    <row r="134" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+      <c r="B134" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E134" s="4" t="s">
+      <c r="E134" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="4" customFormat="1">
-      <c r="A135" s="3"/>
-      <c r="B135" s="3" t="s">
+    <row r="135" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C135" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D135" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E135" s="4" t="s">
+      <c r="E135" s="3" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="4" customFormat="1">
-      <c r="A136" s="3"/>
-      <c r="B136" s="3" t="s">
+    <row r="136" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C136" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D136" s="3" t="s">
+      <c r="D136" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="E136" s="4" t="s">
+      <c r="E136" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="4" customFormat="1">
-      <c r="A137" s="3"/>
-      <c r="B137" s="3" t="s">
+    <row r="137" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
+      <c r="B137" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="C137" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D137" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E137" s="4" t="s">
+      <c r="E137" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="4" customFormat="1">
-      <c r="A138" s="3"/>
-      <c r="B138" s="3" t="s">
+    <row r="138" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+      <c r="B138" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D138" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E138" s="4" t="s">
+      <c r="E138" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="4" customFormat="1">
-      <c r="A139" s="3"/>
-      <c r="B139" s="3" t="s">
+    <row r="139" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
+      <c r="B139" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C139" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D139" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E139" s="4" t="s">
+      <c r="E139" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="4" customFormat="1">
-      <c r="A140" s="3"/>
-      <c r="B140" s="3" t="s">
+    <row r="140" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+      <c r="B140" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D140" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E140" s="4" t="s">
+      <c r="E140" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="4" customFormat="1">
-      <c r="A141" s="3"/>
-      <c r="B141" s="3" t="s">
+    <row r="141" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="C141" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D141" s="3" t="s">
+      <c r="D141" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E141" s="4" t="s">
+      <c r="E141" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="4" customFormat="1">
-      <c r="A142" s="3"/>
-      <c r="B142" s="3" t="s">
+    <row r="142" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+      <c r="B142" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="C142" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D142" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="E142" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="4" customFormat="1">
-      <c r="A143" s="3"/>
-      <c r="B143" s="3" t="s">
+    <row r="143" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+      <c r="B143" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="C143" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D143" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E143" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="4" customFormat="1">
-      <c r="A144" s="3"/>
-      <c r="B144" s="3" t="s">
+    <row r="144" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+      <c r="B144" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E144" s="4" t="s">
+      <c r="E144" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="4" customFormat="1">
-      <c r="A145" s="3"/>
-      <c r="B145" s="3" t="s">
+    <row r="145" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+      <c r="B145" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="C145" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D145" s="3" t="s">
+      <c r="D145" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E145" s="4" t="s">
+      <c r="E145" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="146" spans="1:5" s="4" customFormat="1">
-      <c r="A146" s="3"/>
-      <c r="B146" s="3" t="s">
+    <row r="146" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
+      <c r="B146" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C146" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D146" s="3" t="s">
+      <c r="D146" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E146" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="147" spans="1:5" s="4" customFormat="1">
-      <c r="A147" s="3"/>
-      <c r="B147" s="3" t="s">
+    <row r="147" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="C147" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D147" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E147" s="4" t="s">
+      <c r="E147" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="4" customFormat="1">
-      <c r="A148" s="3"/>
-      <c r="B148" s="3" t="s">
+    <row r="148" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C148" s="4" t="s">
+      <c r="C148" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D148" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E148" s="4" t="s">
+      <c r="E148" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="4" customFormat="1">
-      <c r="A149" s="3"/>
-      <c r="B149" s="3" t="s">
+    <row r="149" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+      <c r="B149" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C149" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D149" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E149" s="4" t="s">
+      <c r="E149" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="150" spans="1:5" s="4" customFormat="1">
-      <c r="A150" s="3"/>
-      <c r="B150" s="3" t="s">
+    <row r="150" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C150" s="4" t="s">
+      <c r="C150" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D150" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="E150" s="4" t="s">
+      <c r="E150" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="4" customFormat="1">
-      <c r="A151" s="3"/>
-      <c r="B151" s="3" t="s">
+    <row r="151" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2"/>
+      <c r="B151" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="C151" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D151" s="3"/>
-      <c r="E151" s="4" t="s">
+      <c r="D151" s="2"/>
+      <c r="E151" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="4" customFormat="1">
-      <c r="A152" s="3"/>
-      <c r="B152" s="3" t="s">
+    <row r="152" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
+      <c r="B152" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="C152" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D152" s="3"/>
-      <c r="E152" s="4" t="s">
+      <c r="D152" s="2"/>
+      <c r="E152" s="3" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="4" customFormat="1">
-      <c r="A153" s="3"/>
-      <c r="B153" s="3" t="s">
+    <row r="153" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C153" s="4" t="s">
+      <c r="C153" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D153" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E153" s="3" t="s">
+      <c r="E153" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="4" customFormat="1">
-      <c r="A154" s="3"/>
-      <c r="B154" s="3" t="s">
+    <row r="154" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2"/>
+      <c r="B154" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C154" s="4" t="s">
+      <c r="C154" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D154" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E154" s="3" t="s">
+      <c r="E154" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
-      <c r="B155" s="2" t="s">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="1" t="s">
         <v>303</v>
       </c>
       <c r="C155" t="s">
@@ -4136,64 +4158,64 @@
         <v>307</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
-      <c r="B156" s="2" t="s">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B156" s="1" t="s">
         <v>305</v>
       </c>
       <c r="C156" t="s">
         <v>304</v>
       </c>
-      <c r="D156" s="2" t="s">
+      <c r="D156" s="1" t="s">
         <v>336</v>
       </c>
       <c r="E156" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
-      <c r="B157" s="2" t="s">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="1" t="s">
         <v>306</v>
       </c>
       <c r="C157" t="s">
         <v>304</v>
       </c>
-      <c r="D157" s="2" t="s">
+      <c r="D157" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E157" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
-      <c r="B158" s="2" t="s">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="1" t="s">
         <v>308</v>
       </c>
       <c r="C158" t="s">
         <v>304</v>
       </c>
-      <c r="D158" s="2" t="s">
+      <c r="D158" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E158" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
-      <c r="B159" s="2" t="s">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="1" t="s">
         <v>312</v>
       </c>
       <c r="C159" t="s">
         <v>304</v>
       </c>
-      <c r="D159" s="2" t="s">
+      <c r="D159" s="1" t="s">
         <v>122</v>
       </c>
       <c r="E159" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
-      <c r="B160" s="2" t="s">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="1" t="s">
         <v>313</v>
       </c>
       <c r="C160" t="s">
@@ -4203,8 +4225,8 @@
         <v>314</v>
       </c>
     </row>
-    <row r="161" spans="2:5">
-      <c r="B161" s="2" t="s">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C161" t="s">
@@ -4214,8 +4236,8 @@
         <v>316</v>
       </c>
     </row>
-    <row r="162" spans="2:5">
-      <c r="B162" s="2" t="s">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="1" t="s">
         <v>317</v>
       </c>
       <c r="C162" t="s">
@@ -4225,8 +4247,8 @@
         <v>319</v>
       </c>
     </row>
-    <row r="163" spans="2:5">
-      <c r="B163" s="2" t="s">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B163" s="1" t="s">
         <v>318</v>
       </c>
       <c r="C163" t="s">
@@ -4236,8 +4258,8 @@
         <v>333</v>
       </c>
     </row>
-    <row r="164" spans="2:5">
-      <c r="B164" s="2" t="s">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B164" s="1" t="s">
         <v>320</v>
       </c>
       <c r="C164" t="s">
@@ -4247,50 +4269,50 @@
         <v>321</v>
       </c>
     </row>
-    <row r="165" spans="2:5">
-      <c r="B165" s="2" t="s">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B165" s="1" t="s">
         <v>322</v>
       </c>
       <c r="C165" t="s">
         <v>199</v>
       </c>
-      <c r="D165" s="2" t="s">
+      <c r="D165" s="1" t="s">
         <v>335</v>
       </c>
       <c r="E165" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="166" spans="2:5">
-      <c r="B166" s="2" t="s">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B166" s="1" t="s">
         <v>326</v>
       </c>
       <c r="C166" t="s">
         <v>199</v>
       </c>
-      <c r="D166" s="2" t="s">
+      <c r="D166" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E166" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="167" spans="2:5">
-      <c r="B167" s="2" t="s">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B167" s="1" t="s">
         <v>328</v>
       </c>
       <c r="C167" t="s">
         <v>199</v>
       </c>
-      <c r="D167" s="2" t="s">
+      <c r="D167" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E167" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="168" spans="2:5">
-      <c r="B168" s="2" t="s">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
         <v>330</v>
       </c>
       <c r="C168" t="s">
@@ -4300,8 +4322,8 @@
         <v>331</v>
       </c>
     </row>
-    <row r="169" spans="2:5">
-      <c r="B169" s="2" t="s">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
         <v>332</v>
       </c>
       <c r="C169" t="s">
@@ -4311,17 +4333,17 @@
         <v>334</v>
       </c>
     </row>
-    <row r="170" spans="2:5">
-      <c r="B170" s="2" t="s">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
         <v>337</v>
       </c>
       <c r="C170" t="s">
         <v>199</v>
       </c>
-      <c r="D170" s="2" t="s">
+      <c r="D170" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E170" s="2" t="s">
+      <c r="E170" s="1" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4332,24 +4354,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Continuation of testing the AdminController. Still not finished
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MovieDbCode\MovieDb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin331221\Desktop\Projects\MovieDbCode\MovieDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1424,7 +1425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1472,12 +1473,6 @@
         <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9966"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1508,8 +1503,11 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1538,11 +1536,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1553,10 +1546,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF9966"/>
       <color rgb="FF99FF99"/>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FFFFFF99"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF6666FF"/>
     </mruColors>
@@ -1861,126 +1853,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="4"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="E1" s="3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="7">
         <v>1</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>3</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>4</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
@@ -1988,13 +1980,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
@@ -2002,13 +1994,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
@@ -2016,13 +2008,13 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>6</v>
       </c>
       <c r="E22" t="s">
@@ -2030,13 +2022,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>8</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -2044,13 +2036,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>9</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="s">
@@ -2058,13 +2050,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E25" t="s">
@@ -2072,13 +2064,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="2">
         <v>8</v>
       </c>
       <c r="E26" t="s">
@@ -2086,13 +2078,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="2">
         <v>11</v>
       </c>
       <c r="E27" t="s">
@@ -2100,13 +2092,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>13</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="2">
         <v>11</v>
       </c>
       <c r="E28" t="s">
@@ -2114,13 +2106,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <v>11</v>
       </c>
       <c r="E29" t="s">
@@ -2128,223 +2120,221 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>15</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="2">
         <v>13</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="20">
         <v>16</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="21" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="23">
         <v>17</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="25" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="23">
         <v>18</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="25" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="25" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="23">
         <v>19</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="25" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
+    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="23">
         <v>20</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="25" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="23">
         <v>21</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="25" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="16">
         <v>22</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9" t="s">
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9" t="s">
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9">
+      <c r="B41" s="2">
         <v>25</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="2">
         <v>6</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
       <c r="B42" s="2">
         <v>26</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>28</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="29" t="s">
+      <c r="E42" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>27</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E43" t="s">
@@ -2352,13 +2342,13 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E44" t="s">
@@ -2366,13 +2356,13 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E45" t="s">
@@ -2380,13 +2370,13 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>30</v>
       </c>
       <c r="C46" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E46" t="s">
@@ -2394,13 +2384,13 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>31</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E47" t="s">
@@ -2408,13 +2398,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>32</v>
       </c>
       <c r="C48" t="s">
         <v>35</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <v>6</v>
       </c>
       <c r="E48" t="s">
@@ -2422,16 +2412,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="18">
         <v>33</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
@@ -2439,16 +2429,16 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>17</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>34</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
@@ -2456,16 +2446,16 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>17</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>35</v>
       </c>
       <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E51" t="s">
@@ -2473,453 +2463,449 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>17</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>36</v>
       </c>
       <c r="C52" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E52" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>6</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="7">
         <v>37</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
         <v>3</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="7">
         <v>38</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
+    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <v>5</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="7">
         <v>39</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="7">
         <v>40</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
+    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>10</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="7">
         <v>41</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="7">
         <v>40</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
+    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>18</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="7">
         <v>42</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
+    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>6</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="7">
         <v>43</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6">
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <v>6</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="7">
         <v>44</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30">
+      <c r="B61" s="2">
         <v>45</v>
       </c>
-      <c r="C61" s="31" t="s">
+      <c r="C61" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="31" t="s">
+      <c r="E61" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30">
+      <c r="B62" s="2">
         <v>46</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C62" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="30" t="s">
+      <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E62" s="31" t="s">
+      <c r="E62" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
-      <c r="B63" s="30">
+      <c r="B63" s="2">
         <v>47</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C63" t="s">
         <v>58</v>
       </c>
-      <c r="D63" s="30" t="s">
+      <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="31" t="s">
+      <c r="E63" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30">
+      <c r="B64" s="2">
         <v>48</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" t="s">
         <v>58</v>
       </c>
-      <c r="D64" s="30" t="s">
+      <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="31" t="s">
+      <c r="E64" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="7">
         <v>49</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="7">
         <v>50</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E66" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="7">
         <v>51</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="E68" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="E69" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C70" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E75" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D77" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E77" s="7" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="3" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2930,7 +2916,7 @@
       <c r="B79" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" t="s">
         <v>58</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -2947,7 +2933,7 @@
       <c r="B80" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" t="s">
         <v>58</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -2958,36 +2944,36 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="30" t="s">
+      <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B81" s="30" t="s">
+      <c r="B81" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C81" s="31" t="s">
+      <c r="C81" t="s">
         <v>58</v>
       </c>
-      <c r="D81" s="30" t="s">
+      <c r="D81" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E81" s="30" t="s">
+      <c r="E81" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="30" t="s">
+      <c r="A82" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="30" t="s">
+      <c r="B82" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C82" s="31" t="s">
+      <c r="C82" t="s">
         <v>58</v>
       </c>
-      <c r="D82" s="30" t="s">
+      <c r="D82" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E82" s="30" t="s">
+      <c r="E82" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2998,7 +2984,7 @@
       <c r="B83" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" t="s">
         <v>58</v>
       </c>
       <c r="D83" s="2" t="s">
@@ -3015,7 +3001,7 @@
       <c r="B84" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" t="s">
         <v>58</v>
       </c>
       <c r="D84" s="2" t="s">
@@ -3025,1130 +3011,1130 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D85" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="E85" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="D86" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="E86" s="11" t="s">
+      <c r="E86" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D87" s="6" t="s">
+      <c r="D87" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E87" s="6" t="s">
+      <c r="E87" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E88" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D89" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D90" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="E90" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D91" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D92" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="E92" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D93" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="E93" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D94" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="E94" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E96" s="2" t="s">
+      <c r="E96" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D97" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="E97" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D98" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="E98" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D99" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="E99" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E101" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="E102" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D103" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="E103" s="3" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E104" s="2" t="s">
+      <c r="E104" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E105" s="2" t="s">
+      <c r="E105" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E106" s="2" t="s">
+      <c r="E106" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D107" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="E107" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D108" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E108" s="2" t="s">
+      <c r="E108" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D109" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="E109" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D110" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E110" s="2" t="s">
+      <c r="E110" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="D111" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="E111" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D112" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E112" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D113" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E113" s="2" t="s">
+      <c r="E113" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C115" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D115" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E115" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="E116" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D117" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="E117" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C118" s="12" t="s">
+      <c r="C118" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D118" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E118" s="2" t="s">
+      <c r="E118" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="6" t="s">
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B119" s="6" t="s">
+      <c r="B119" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="6" t="s">
+      <c r="D119" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E119" s="6" t="s">
+      <c r="E119" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B120" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C120" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D120" s="6" t="s">
+      <c r="D120" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E120" s="6" t="s">
+      <c r="E120" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D121" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E121" s="2" t="s">
+      <c r="E121" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C122" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E122" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D123" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E123" s="2" t="s">
+      <c r="E123" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="25" t="s">
+    <row r="124" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="B124" s="25" t="s">
+      <c r="B124" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="C124" s="26" t="s">
+      <c r="C124" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D124" s="25" t="s">
+      <c r="D124" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="E124" s="25" t="s">
+      <c r="E124" s="26" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="27"/>
-      <c r="B125" s="27" t="s">
+    <row r="125" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="28"/>
+      <c r="B125" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="C125" s="28" t="s">
+      <c r="C125" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D125" s="27"/>
-      <c r="E125" s="28" t="s">
+      <c r="D125" s="28"/>
+      <c r="E125" s="29" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2" t="s">
+    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="C126" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D126" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E126" s="3" t="s">
+      <c r="E126" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2" t="s">
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C127" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D127" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E127" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2" t="s">
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C128" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="D128" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E128" s="3" t="s">
+      <c r="E128" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2" t="s">
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="C129" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D129" s="2"/>
-      <c r="E129" s="3" t="s">
+      <c r="D129" s="3"/>
+      <c r="E129" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2" t="s">
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C130" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D130" s="2" t="s">
+      <c r="D130" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E130" s="3" t="s">
+      <c r="E130" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2" t="s">
+    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C131" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D131" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E131" s="3" t="s">
+      <c r="E131" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2" t="s">
+    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="C132" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="D132" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E132" s="3" t="s">
+      <c r="E132" s="4" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="6"/>
-      <c r="B133" s="6" t="s">
+    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="C133" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D133" s="6" t="s">
+      <c r="D133" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="E133" s="7" t="s">
+      <c r="E133" s="8" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2" t="s">
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C134" s="3" t="s">
+      <c r="C134" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="D134" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E134" s="3" t="s">
+      <c r="E134" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2" t="s">
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C135" s="3" t="s">
+      <c r="C135" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="D135" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E135" s="3" t="s">
+      <c r="E135" s="4" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2" t="s">
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C136" s="3" t="s">
+      <c r="C136" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D136" s="2" t="s">
+      <c r="D136" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E136" s="3" t="s">
+      <c r="E136" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2" t="s">
+    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="C137" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D137" s="2" t="s">
+      <c r="D137" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E137" s="3" t="s">
+      <c r="E137" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2" t="s">
+    <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C138" s="3" t="s">
+      <c r="C138" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="D138" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E138" s="3" t="s">
+      <c r="E138" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2" t="s">
+    <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="C139" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="D139" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E139" s="3" t="s">
+      <c r="E139" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2" t="s">
+    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="C140" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="D140" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E140" s="3" t="s">
+      <c r="E140" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2" t="s">
+    <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C141" s="3" t="s">
+      <c r="C141" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D141" s="2" t="s">
+      <c r="D141" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E141" s="3" t="s">
+      <c r="E141" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2" t="s">
+    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C142" s="3" t="s">
+      <c r="C142" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="D142" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E142" s="3" t="s">
+      <c r="E142" s="4" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2" t="s">
+    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C143" s="3" t="s">
+      <c r="C143" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D143" s="2" t="s">
+      <c r="D143" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E143" s="3" t="s">
+      <c r="E143" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2" t="s">
+    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C144" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D144" s="2" t="s">
+      <c r="D144" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="E144" s="3" t="s">
+      <c r="E144" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2" t="s">
+    <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C145" s="3" t="s">
+      <c r="C145" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D145" s="2" t="s">
+      <c r="D145" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E145" s="3" t="s">
+      <c r="E145" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="146" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2" t="s">
+    <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C146" s="3" t="s">
+      <c r="C146" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D146" s="2" t="s">
+      <c r="D146" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E146" s="3" t="s">
+      <c r="E146" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="147" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2" t="s">
+    <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C147" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D147" s="2" t="s">
+      <c r="D147" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E147" s="3" t="s">
+      <c r="E147" s="4" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2" t="s">
+    <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C148" s="3" t="s">
+      <c r="C148" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D148" s="2" t="s">
+      <c r="D148" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E148" s="3" t="s">
+      <c r="E148" s="4" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2" t="s">
+    <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C149" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D149" s="2" t="s">
+      <c r="D149" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="E149" s="3" t="s">
+      <c r="E149" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="150" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2" t="s">
+    <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="C150" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D150" s="2" t="s">
+      <c r="D150" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E150" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2" t="s">
+    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C151" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D151" s="2"/>
-      <c r="E151" s="3" t="s">
+      <c r="D151" s="3"/>
+      <c r="E151" s="4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="2"/>
-      <c r="B152" s="2" t="s">
+    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C152" s="3" t="s">
+      <c r="C152" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D152" s="2"/>
-      <c r="E152" s="3" t="s">
+      <c r="D152" s="3"/>
+      <c r="E152" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="2"/>
-      <c r="B153" s="2" t="s">
+    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C153" s="3" t="s">
+      <c r="C153" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D153" s="2" t="s">
+      <c r="D153" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E153" s="2" t="s">
+      <c r="E153" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2" t="s">
+    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C154" s="3" t="s">
+      <c r="C154" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D154" s="2" t="s">
+      <c r="D154" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E154" s="2" t="s">
+      <c r="E154" s="3" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="2" t="s">
         <v>303</v>
       </c>
       <c r="C155" t="s">
@@ -4159,13 +4145,13 @@
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C156" t="s">
         <v>304</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D156" s="2" t="s">
         <v>336</v>
       </c>
       <c r="E156" t="s">
@@ -4173,13 +4159,13 @@
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="2" t="s">
         <v>306</v>
       </c>
       <c r="C157" t="s">
         <v>304</v>
       </c>
-      <c r="D157" s="1" t="s">
+      <c r="D157" s="2" t="s">
         <v>104</v>
       </c>
       <c r="E157" t="s">
@@ -4187,13 +4173,13 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="2" t="s">
         <v>308</v>
       </c>
       <c r="C158" t="s">
         <v>304</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="D158" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E158" t="s">
@@ -4201,13 +4187,13 @@
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="2" t="s">
         <v>312</v>
       </c>
       <c r="C159" t="s">
         <v>304</v>
       </c>
-      <c r="D159" s="1" t="s">
+      <c r="D159" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E159" t="s">
@@ -4215,7 +4201,7 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="2" t="s">
         <v>313</v>
       </c>
       <c r="C160" t="s">
@@ -4226,7 +4212,7 @@
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="2" t="s">
         <v>315</v>
       </c>
       <c r="C161" t="s">
@@ -4237,7 +4223,7 @@
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="2" t="s">
         <v>317</v>
       </c>
       <c r="C162" t="s">
@@ -4248,7 +4234,7 @@
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="2" t="s">
         <v>318</v>
       </c>
       <c r="C163" t="s">
@@ -4259,7 +4245,7 @@
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="2" t="s">
         <v>320</v>
       </c>
       <c r="C164" t="s">
@@ -4270,13 +4256,13 @@
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="2" t="s">
         <v>322</v>
       </c>
       <c r="C165" t="s">
         <v>199</v>
       </c>
-      <c r="D165" s="1" t="s">
+      <c r="D165" s="2" t="s">
         <v>335</v>
       </c>
       <c r="E165" t="s">
@@ -4284,13 +4270,13 @@
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="2" t="s">
         <v>326</v>
       </c>
       <c r="C166" t="s">
         <v>199</v>
       </c>
-      <c r="D166" s="1" t="s">
+      <c r="D166" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E166" t="s">
@@ -4298,13 +4284,13 @@
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="2" t="s">
         <v>328</v>
       </c>
       <c r="C167" t="s">
         <v>199</v>
       </c>
-      <c r="D167" s="1" t="s">
+      <c r="D167" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E167" t="s">
@@ -4312,7 +4298,7 @@
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="2" t="s">
         <v>330</v>
       </c>
       <c r="C168" t="s">
@@ -4323,7 +4309,7 @@
       </c>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="2" t="s">
         <v>332</v>
       </c>
       <c r="C169" t="s">
@@ -4334,16 +4320,16 @@
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B170" s="1" t="s">
+      <c r="B170" s="2" t="s">
         <v>337</v>
       </c>
       <c r="C170" t="s">
         <v>199</v>
       </c>
-      <c r="D170" s="1" t="s">
+      <c r="D170" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E170" s="1" t="s">
+      <c r="E170" s="2" t="s">
         <v>338</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Forgot to push function requirements document in last commit.
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin331221\Desktop\Projects\MovieDbCode\MovieDb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MovieDbCode\MovieDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -97,9 +96,6 @@
   </si>
   <si>
     <t>Receive a notification when a user comments on a review.</t>
-  </si>
-  <si>
-    <t>Controller that properly deletes a person, and all corresponding person information from the database.</t>
   </si>
   <si>
     <t>Add bootstrap search bar to menu bar</t>
@@ -1229,9 +1225,6 @@
     <t>Page to create a Person. Form has all fields for person info (first name, middle name, last name, first alias, middle alias, last alias, country of birth, date of birth, date of death, biography).</t>
   </si>
   <si>
-    <t>Controller that properly deletes a movie, and all corresponding movie information from the database (includes reviews, and discussions).</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -1374,6 +1367,12 @@
   </si>
   <si>
     <t>If a user attempts to display a review that does not exist, a review not found page is displayed.</t>
+  </si>
+  <si>
+    <t>Controller that properly deletes a movie, and all corresponding movie information from the database (includes reviews, discussions and album/images).</t>
+  </si>
+  <si>
+    <t>Controller that properly deletes a person, and all corresponding person information from the database (including album/images).</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1502,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1520,10 +1519,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1854,7 +1850,7 @@
   <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,37 +1865,37 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="15" t="s">
-        <v>285</v>
+      <c r="E6" s="14" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1916,7 +1912,7 @@
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -1933,7 +1929,7 @@
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1942,15 +1938,15 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -1959,10 +1955,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,7 +2028,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2046,7 +2042,7 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2133,146 +2129,146 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="B31" s="20">
+    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" s="17">
         <v>16</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" s="20">
+        <v>17</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="22" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B32" s="23">
-        <v>17</v>
-      </c>
-      <c r="C32" s="24" t="s">
+    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="20">
+        <v>18</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D33" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E33" s="22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" s="20">
+        <v>19</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B33" s="23">
-        <v>18</v>
-      </c>
-      <c r="C33" s="24" t="s">
+    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B36" s="20">
+        <v>20</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="25" t="s">
+      <c r="D36" s="19" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="C34" s="25" t="s">
+      <c r="E36" s="22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37" s="20">
+        <v>21</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="25" t="s">
+      <c r="D37" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B35" s="23">
-        <v>19</v>
-      </c>
-      <c r="C35" s="24" t="s">
+      <c r="B38" s="20">
+        <v>22</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B36" s="23">
-        <v>20</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="B37" s="23">
-        <v>21</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="B38" s="16">
-        <v>22</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>25</v>
+      <c r="D38" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>4</v>
@@ -2281,13 +2277,13 @@
         <v>6</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>4</v>
@@ -2296,7 +2292,7 @@
         <v>6</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2304,13 +2300,13 @@
         <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="2">
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2318,13 +2314,13 @@
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2335,10 +2331,10 @@
         <v>13</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2349,10 +2345,10 @@
         <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,13 +2356,13 @@
         <v>29</v>
       </c>
       <c r="C45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
         <v>35</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,13 +2370,13 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2388,13 +2384,13 @@
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2402,30 +2398,30 @@
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="2">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="18">
+      <c r="B49" s="15">
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,7 +2438,7 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,7 +2455,7 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,7 +2472,7 @@
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2487,13 +2483,13 @@
         <v>37</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2504,13 +2500,13 @@
         <v>38</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2521,30 +2517,30 @@
         <v>39</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B56" s="7">
         <v>40</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2555,13 +2551,13 @@
         <v>41</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D57" s="7">
         <v>40</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2572,13 +2568,13 @@
         <v>42</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2589,13 +2585,13 @@
         <v>43</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2606,13 +2602,13 @@
         <v>44</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D60" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2620,13 +2616,13 @@
         <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,13 +2630,13 @@
         <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2648,13 +2644,13 @@
         <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2662,786 +2658,786 @@
         <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="7">
         <v>49</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="7">
         <v>50</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="7">
         <v>51</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D67" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="C68" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="7" t="s">
+      <c r="E68" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B69" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="E69" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C70" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D75" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="D77" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="E77" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E78" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C80" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C80" t="s">
-        <v>58</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E80" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C81" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E81" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C82" t="s">
-        <v>58</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E82" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C83" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C84" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C84" t="s">
-        <v>58</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="C85" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E86" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>122</v>
-      </c>
       <c r="C87" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>4</v>
@@ -3450,15 +3446,15 @@
         <v>6</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>4</v>
@@ -3467,134 +3463,134 @@
         <v>6</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="C115" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B116" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="C116" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D116" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B117" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D117" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C118" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D118" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>4</v>
@@ -3603,15 +3599,15 @@
         <v>6</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>4</v>
@@ -3620,717 +3616,717 @@
         <v>6</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="C123" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D123" s="3" t="s">
+      <c r="E123" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E123" s="3" t="s">
+    </row>
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B124" s="23" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="26" t="s">
+      <c r="C124" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="B124" s="26" t="s">
+      <c r="E124" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="C124" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D124" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="E124" s="26" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="28"/>
-      <c r="B125" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="C125" s="29" t="s">
+    </row>
+    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="25"/>
+      <c r="B125" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C125" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D125" s="28"/>
-      <c r="E125" s="29" t="s">
-        <v>301</v>
+      <c r="D125" s="25"/>
+      <c r="E125" s="26" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E138" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E139" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E140" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E141" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D142" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E142" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D143" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E143" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="E143" s="4" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D151" s="3"/>
       <c r="E151" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D152" s="3"/>
       <c r="E152" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B155" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C155" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E155" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C156" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E156" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C157" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E157" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B158" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C158" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E158" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B159" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C159" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E159" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C160" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E160" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C161" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E161" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C162" t="s">
+        <v>302</v>
+      </c>
+      <c r="E162" t="s">
         <v>317</v>
-      </c>
-      <c r="C162" t="s">
-        <v>304</v>
-      </c>
-      <c r="E162" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C163" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E163" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B164" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C164" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E164" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B165" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C165" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E165" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B166" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C166" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E166" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B167" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C167" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E167" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B168" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C168" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E168" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C169" t="s">
+        <v>198</v>
+      </c>
+      <c r="E169" t="s">
         <v>332</v>
-      </c>
-      <c r="C169" t="s">
-        <v>199</v>
-      </c>
-      <c r="E169" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B170" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C170" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added integration and acceptance tests for movie and people pages.
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MovieDbCode\MovieDb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\Projects\MovieDbCode\MovieDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1424,7 +1424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1472,6 +1472,12 @@
         <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1502,7 +1508,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1532,6 +1538,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1542,9 +1550,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFF99FF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF6666FF"/>
     </mruColors>
@@ -1849,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,31 +2025,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
+    <row r="24" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27">
         <v>9</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="28" t="s">
         <v>308</v>
       </c>
     </row>
@@ -4129,96 +4139,106 @@
         <v>298</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B155" s="2" t="s">
+    <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="E155" t="s">
+      <c r="D155" s="3"/>
+      <c r="E155" s="4" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="2" t="s">
+    <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D156" s="2" t="s">
+      <c r="D156" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="4" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B157" s="2" t="s">
+    <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D157" s="2" t="s">
+      <c r="D157" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B158" s="2" t="s">
+    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D158" s="2" t="s">
+      <c r="D158" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="4" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B159" s="2" t="s">
+    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3"/>
+      <c r="B159" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D159" s="2" t="s">
+      <c r="D159" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B160" s="2" t="s">
+    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="E160" t="s">
+      <c r="D160" s="3"/>
+      <c r="E160" s="4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="2" t="s">
+    <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="3"/>
+      <c r="B161" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="E161" t="s">
+      <c r="D161" s="3"/>
+      <c r="E161" s="4" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
         <v>315</v>
       </c>
@@ -4229,7 +4249,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
         <v>316</v>
       </c>
@@ -4240,71 +4260,78 @@
         <v>331</v>
       </c>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B164" s="2" t="s">
+    <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="3"/>
+      <c r="B164" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E164" t="s">
+      <c r="D164" s="3"/>
+      <c r="E164" s="4" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B165" s="2" t="s">
+    <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D165" s="2" t="s">
+      <c r="D165" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B166" s="2" t="s">
+    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="3"/>
+      <c r="B166" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D166" s="2" t="s">
+      <c r="D166" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="4" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B167" s="2" t="s">
+    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="3"/>
+      <c r="B167" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D167" s="2" t="s">
+      <c r="D167" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B168" s="2" t="s">
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E168" t="s">
+      <c r="D168" s="3"/>
+      <c r="E168" s="4" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
         <v>330</v>
       </c>
@@ -4315,17 +4342,18 @@
         <v>332</v>
       </c>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B170" s="2" t="s">
+    <row r="170" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="27"/>
+      <c r="B170" s="27" t="s">
         <v>335</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="D170" s="2" t="s">
+      <c r="D170" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="E170" s="2" t="s">
+      <c r="E170" s="27" t="s">
         <v>336</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated reqs for Tim to continue updating
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Projects\MovieDb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\Projects\MovieDbCode\MovieDb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="80" windowWidth="12440" windowHeight="6230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="341">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -96,15 +96,6 @@
   </si>
   <si>
     <t>Receive a notification when a user comments on a review.</t>
-  </si>
-  <si>
-    <t>View and Controller for displaying associated person info, i.e. What roles they've had in movies, and other biographic information. Links for admin to Edit or Delete person.</t>
-  </si>
-  <si>
-    <t>View and Controller for displaying associated movie info. Reviews and comments are displayed on the page below the movie info. Links for admin to Edit or Delete movie.</t>
-  </si>
-  <si>
-    <t>Controller that properly deletes a person, and all corresponding person information from the database.</t>
   </si>
   <si>
     <t>Add bootstrap search bar to menu bar</t>
@@ -1051,9 +1042,6 @@
     <t>109</t>
   </si>
   <si>
-    <t>A review can be created for any existing movie through a review creation page.</t>
-  </si>
-  <si>
     <t>110</t>
   </si>
   <si>
@@ -1111,9 +1099,6 @@
     <t>119</t>
   </si>
   <si>
-    <t>The user information section contains buttons for deleting and editing a review.</t>
-  </si>
-  <si>
     <t>120</t>
   </si>
   <si>
@@ -1219,9 +1204,6 @@
     <t>136</t>
   </si>
   <si>
-    <t>If a user attempts to display a review that does no exist, a review not found page is displayed.</t>
-  </si>
-  <si>
     <t>TESTING IN PROGRESS</t>
   </si>
   <si>
@@ -1243,9 +1225,6 @@
     <t>Page to create a Person. Form has all fields for person info (first name, middle name, last name, first alias, middle alias, last alias, country of birth, date of birth, date of death, biography).</t>
   </si>
   <si>
-    <t>Controller that properly deletes a movie, and all corresponding movie information from the database (includes reviews, and discussions).</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -1258,95 +1237,149 @@
     <t>7</t>
   </si>
   <si>
-    <t>Clicking the forgot password button take the user to a page to recover their password</t>
-  </si>
-  <si>
-    <t>Checking the "remember me" saves the user's credentials for login</t>
-  </si>
-  <si>
-    <t>Be able to log in the website directly from the landing page</t>
-  </si>
-  <si>
-    <t>Be able to register an account directly on the landing page</t>
-  </si>
-  <si>
-    <t>Provide a list of the top 10 movies of the month</t>
-  </si>
-  <si>
-    <t>Provide clickable links to the movie pages in the top 10 movies of the month list</t>
-  </si>
-  <si>
-    <t>Provide a list of the top 10 recently released movies</t>
-  </si>
-  <si>
-    <t>Provide clickable links to the movie pages in the recently released movie list</t>
-  </si>
-  <si>
-    <t>Provide a list of 3 recently added reviews to any movie</t>
-  </si>
-  <si>
-    <t>Allow user to click "see full review" to be taken to that review's page</t>
-  </si>
-  <si>
-    <t>If a user is logged in, the login and register boxes are not to be displayed</t>
-  </si>
-  <si>
-    <t>Provide a navigation bar, with search, advanced search, and links to the home page, user page, login and register pages</t>
-  </si>
-  <si>
     <t>137</t>
   </si>
   <si>
+    <t>A user can only create one review per movie.</t>
+  </si>
+  <si>
     <t>138</t>
   </si>
   <si>
+    <t>The delete review button deletes a review, as well as the comments and votes associated with it.</t>
+  </si>
+  <si>
+    <t>A review creation page exists which is used to create reviews.</t>
+  </si>
+  <si>
+    <t>The user information section contains buttons for deleting and editing a review when the user is logged in.</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
     <t>140</t>
   </si>
   <si>
-    <t>139</t>
-  </si>
-  <si>
     <t>141</t>
   </si>
   <si>
+    <t>There are two buttons, "edit movie" and "delete movie" that only appear when an admin is logged in.</t>
+  </si>
+  <si>
     <t>142</t>
   </si>
   <si>
+    <t>Movie page view/controller displays the correct information on the movie blade: title, year, release date, director, runtime, parental rating, synopsis, genre, country, and movie poster.</t>
+  </si>
+  <si>
+    <t>Person page view/controller displays the correct information on the person blade: First name, middle name, last name, first alias, middle alias, last alias,  country of origin, date of birth, date of death, biography and picture.</t>
+  </si>
+  <si>
+    <t>The pictures section of a movie page contains a partial view of the album associated with the movie. The max amount of images is 8.</t>
+  </si>
+  <si>
     <t>143</t>
   </si>
   <si>
     <t>144</t>
   </si>
   <si>
+    <t>The cast section of a movie page displays a table containing each cast member's full name, their pictures, and their role in the movie.</t>
+  </si>
+  <si>
     <t>145</t>
   </si>
   <si>
+    <t>The crew section of a movie page displays a table containing each crew member's full name, their pictures, and their role in the crew.</t>
+  </si>
+  <si>
     <t>146</t>
   </si>
   <si>
     <t>147</t>
   </si>
   <si>
+    <t>The reviews sections of a movie page displays a partial view of reviews related to the movie.</t>
+  </si>
+  <si>
     <t>148</t>
   </si>
   <si>
-    <t>6, 33</t>
-  </si>
-  <si>
-    <t>33, 8</t>
-  </si>
-  <si>
-    <t>33,8</t>
-  </si>
-  <si>
-    <t>33, 109</t>
+    <t>There are two buttons, "edit person" and "delete person" that only appear when an admin is logged in.</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>There is an admin button "delete movie" that redirects to the admin's delete movie page.</t>
+  </si>
+  <si>
+    <t>There is an admin button "edit movie" that redirects to the admin's edit movie page.</t>
+  </si>
+  <si>
+    <t>There is an admin button "delete person" that redirects to the admin's delete person page.</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>There is an admin button "edit person" that redirects to the admin's edit person page.</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>The pictures section of a person page contains a partial view of the album associated with the person. The max amount of images is 8.</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>The filmography section of a person page displays a table containing each movie the person is associated with, their role in the movie, and the movie poster for the movie.</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>The discussions section of a movie page displays a partial view of discussions related to the movie.</t>
+  </si>
+  <si>
+    <t>The discussions section of a person page displays a partial view of discussions associated with that person.</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>The pictures section of a person page contains a button "view all pictures" that redirects a person to an album preview page.</t>
+  </si>
+  <si>
+    <t>The pictures section of a movie page contains a button "view all pictures" that redirects a person to an album preview page.</t>
+  </si>
+  <si>
+    <t>If a user attempts to display a review that does not exist, a review not found page is displayed.</t>
+  </si>
+  <si>
+    <t>Controller that properly deletes a movie, and all corresponding movie information from the database (includes reviews, discussions and album/images).</t>
+  </si>
+  <si>
+    <t>Controller that properly deletes a person, and all corresponding person information from the database (including album/images).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1383,8 +1416,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1421,6 +1461,17 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FF99"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1446,11 +1497,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1467,10 +1519,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1479,9 +1528,14 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1489,8 +1543,8 @@
   <colors>
     <mruColors>
       <color rgb="FF99FF99"/>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFF99FF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF6666FF"/>
     </mruColors>
@@ -1793,55 +1847,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="208.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E4" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E6" s="15" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1856,9 +1910,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -1873,9 +1927,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1884,15 +1938,15 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -1901,13 +1955,13 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -1921,7 +1975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -1935,7 +1989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -1949,7 +2003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -1963,35 +2017,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="2">
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="2">
+      <c r="E23" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3">
         <v>9</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -2005,7 +2061,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -2019,7 +2075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -2033,7 +2089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -2047,7 +2103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -2061,7 +2117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -2075,146 +2131,146 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="B31" s="20">
+    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" s="17">
         <v>16</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" s="20">
+        <v>17</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="20">
+        <v>18</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="B32" s="23">
-        <v>17</v>
-      </c>
-      <c r="C32" s="24" t="s">
+    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" s="20">
+        <v>19</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="B33" s="23">
-        <v>18</v>
-      </c>
-      <c r="C33" s="24" t="s">
+      <c r="D35" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B36" s="20">
+        <v>20</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="C34" s="25" t="s">
+      <c r="D36" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37" s="20">
+        <v>21</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="B35" s="23">
-        <v>19</v>
-      </c>
-      <c r="C35" s="24" t="s">
+      <c r="D37" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B38" s="20">
+        <v>22</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>291</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="B36" s="23">
-        <v>20</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>298</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="B37" s="16">
-        <v>21</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="B38" s="16">
-        <v>22</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>4</v>
@@ -2223,13 +2279,13 @@
         <v>6</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>4</v>
@@ -2238,38 +2294,38 @@
         <v>6</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D41" s="2">
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2277,13 +2333,13 @@
         <v>13</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2291,86 +2347,86 @@
         <v>14</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>31</v>
       </c>
       <c r="C47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D48" s="2">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="18">
+      <c r="B49" s="15">
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2384,10 +2440,10 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>17</v>
       </c>
@@ -2401,10 +2457,10 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>17</v>
       </c>
@@ -2418,10 +2474,10 @@
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2429,16 +2485,16 @@
         <v>37</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2446,16 +2502,16 @@
         <v>38</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2463,33 +2519,33 @@
         <v>39</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B56" s="7">
         <v>40</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2497,16 +2553,16 @@
         <v>41</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D57" s="7">
         <v>40</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2514,16 +2570,16 @@
         <v>42</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2531,16 +2587,16 @@
         <v>43</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2548,842 +2604,842 @@
         <v>44</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B65" s="7">
         <v>49</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B66" s="7">
         <v>50</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B67" s="7">
         <v>51</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D67" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="B68" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="7" t="s">
+      <c r="C68" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="7" t="s">
+    </row>
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D68" s="7" t="s">
+      <c r="C69" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E69" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" s="7" t="s">
+      <c r="C70" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D69" s="7" t="s">
+      <c r="E70" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E69" s="7" t="s">
+    </row>
+    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C70" t="s">
-        <v>65</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76" s="3" t="s">
+      <c r="E78" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C80" t="s">
+        <v>57</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C83" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C84" t="s">
+        <v>57</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C79" t="s">
-        <v>60</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C80" t="s">
-        <v>60</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C81" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C82" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C83" t="s">
-        <v>60</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C84" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E84" s="2" t="s">
+      <c r="D85" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="12" t="s">
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E85" s="12" t="s">
+      <c r="C86" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E86" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="12" t="s">
+    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="C87" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="E86" s="12" t="s">
+      <c r="B88" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="7" t="s">
+      <c r="C88" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E89" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E87" s="7" t="s">
+    </row>
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="B90" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>4</v>
@@ -3392,15 +3448,15 @@
         <v>6</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>4</v>
@@ -3409,134 +3465,134 @@
         <v>6</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E112" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B113" s="3" t="s">
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E113" s="3" t="s">
+      <c r="B115" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A115" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B115" s="3" t="s">
+      <c r="C115" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C115" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D115" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D116" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="E116" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D116" s="3" t="s">
+    </row>
+    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="C117" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B117" s="3" t="s">
+      <c r="E117" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B118" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D117" s="3" t="s">
+      <c r="C118" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B118" s="3" t="s">
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B119" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>4</v>
@@ -3545,15 +3601,15 @@
         <v>6</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>4</v>
@@ -3562,623 +3618,735 @@
         <v>6</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B123" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="C123" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B123" s="3" t="s">
+      <c r="E123" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B124" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="C123" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D123" s="3" t="s">
+      <c r="C124" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E124" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="E123" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B125" s="2" t="s">
+    </row>
+    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="25"/>
+      <c r="B125" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C125" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125" s="25"/>
+      <c r="E125" s="26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C127" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E125" t="s">
+      <c r="D127" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E127" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B126" s="2" t="s">
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C128" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="D128" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E128" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B127" s="2" t="s">
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="D129" s="3"/>
+      <c r="E129" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B128" s="2" t="s">
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C130" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E128" t="s">
+      <c r="D130" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E130" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B129" s="2" t="s">
+    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C131" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E129" t="s">
+      <c r="D131" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E131" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B130" s="2" t="s">
+    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C132" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="D132" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E132" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B131" s="2" t="s">
+    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C133" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E131" t="s">
+      <c r="D133" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E133" s="8" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B132" s="2" t="s">
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C134" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D132" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E132" t="s">
+      <c r="D134" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E134" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B133" s="2" t="s">
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C135" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E133" t="s">
+      <c r="D135" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B134" s="2" t="s">
+      <c r="C136" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E136" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C134" t="s">
+    </row>
+    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C137" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E134" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B135" s="2" t="s">
+      <c r="D137" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E137" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C135" t="s">
+    </row>
+    <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C138" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E135" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B136" s="2" t="s">
+      <c r="D138" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E138" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C136" t="s">
+    </row>
+    <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C139" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E136" t="s">
+      <c r="D139" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141" s="3" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B137" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C137" t="s">
+      <c r="E141" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C142" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D137" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E137" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B138" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C138" t="s">
+      <c r="D142" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C143" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D138" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E138" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B139" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="D143" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C144" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D139" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E139" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B140" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="D144" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C145" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E140" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B141" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C141" t="s">
+      <c r="D145" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C146" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D141" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E141" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B142" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C142" t="s">
+      <c r="D146" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C147" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D142" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E142" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B143" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C143" t="s">
+      <c r="D147" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C148" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D143" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E143" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B144" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="D148" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C149" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D144" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E144" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B145" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C145" t="s">
+      <c r="D149" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C150" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D145" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E145" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B146" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C146" t="s">
+      <c r="D150" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C151" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D146" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E146" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B147" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C147" t="s">
+      <c r="D151" s="3"/>
+      <c r="E151" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C152" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D147" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E147" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B148" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C148" t="s">
+      <c r="D152" s="3"/>
+      <c r="E152" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C153" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D148" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E148" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B149" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C149" t="s">
+      <c r="D153" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C154" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D149" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E149" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B150" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="C150" t="s">
-        <v>15</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E150" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B151" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C151" t="s">
-        <v>15</v>
-      </c>
-      <c r="E151" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B152" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C152" t="s">
-        <v>15</v>
-      </c>
-      <c r="E152" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B153" s="2" t="s">
+      <c r="D154" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D155" s="3"/>
+      <c r="E155" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3"/>
+      <c r="B159" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D160" s="3"/>
+      <c r="E160" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="3"/>
+      <c r="B161" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D161" s="3"/>
+      <c r="E161" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="C153" t="s">
-        <v>44</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E153" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B154" s="2" t="s">
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C154" t="s">
-        <v>44</v>
-      </c>
-      <c r="D154" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E154" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B155" s="2" t="s">
+      <c r="C162" t="s">
+        <v>302</v>
+      </c>
+      <c r="E162" t="s">
         <v>317</v>
       </c>
-      <c r="C155" t="s">
-        <v>44</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E155" t="s">
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B163" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C163" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B156" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C156" t="s">
-        <v>44</v>
-      </c>
-      <c r="D156" s="2" t="s">
+      <c r="E163" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="3"/>
+      <c r="B164" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D164" s="3"/>
+      <c r="E164" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="3"/>
+      <c r="B166" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="3"/>
+      <c r="B167" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E156" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B157" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C157" t="s">
-        <v>44</v>
-      </c>
-      <c r="D157" s="2" t="s">
+      <c r="C167" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="E157" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B158" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C158" t="s">
-        <v>44</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E158" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B159" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C159" t="s">
-        <v>44</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E159" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B160" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C160" t="s">
-        <v>44</v>
-      </c>
-      <c r="D160" s="2" t="s">
+    </row>
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E160" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B161" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C161" t="s">
-        <v>44</v>
-      </c>
-      <c r="D161" s="2" t="s">
+      <c r="C168" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D168" s="3"/>
+      <c r="E168" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="E161" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B162" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C162" t="s">
-        <v>44</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E162" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B163" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C163" t="s">
-        <v>44</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E163" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B164" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C164" t="s">
-        <v>44</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E164" t="s">
-        <v>313</v>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B169" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C169" t="s">
+        <v>198</v>
+      </c>
+      <c r="E169" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="3"/>
+      <c r="B170" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -4193,7 +4361,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4205,7 +4373,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented discussion board component on movie and landing page. Updated functional req and test manual for Discussions
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytonjohnson/Desktop/Projects/MovieDbCode/MovieDb/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="12435" windowHeight="6225"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="17680" windowHeight="13700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="314">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -1264,12 +1274,36 @@
   <si>
     <t>The user information section contains buttons for deleting and editing a review when the user is logged in.</t>
   </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>The post a reply button should redirect user to Reply creation page.</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Navigating to ./discussions/create/{mid} should take user to discussion creation page.</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>Discussion creation form should be properly saved to the database.</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>Most recent discussions should appear on landing page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1496,12 +1530,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1528,14 +1562,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1562,6 +1597,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1737,54 +1773,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="208.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" s="15" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1801,7 +1837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>130</v>
       </c>
@@ -1818,7 +1854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>131</v>
       </c>
@@ -1835,7 +1871,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>132</v>
       </c>
@@ -1852,7 +1888,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -1866,7 +1902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -1880,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -1894,7 +1930,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -1908,7 +1944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>8</v>
       </c>
@@ -1922,7 +1958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -1936,7 +1972,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -1950,7 +1986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -1964,7 +2000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -1978,7 +2014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -1992,7 +2028,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -2006,7 +2042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -2020,7 +2056,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1">
+    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>299</v>
       </c>
@@ -2037,7 +2073,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="24" customFormat="1">
+    <row r="32" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>299</v>
       </c>
@@ -2054,7 +2090,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="24" customFormat="1">
+    <row r="33" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>299</v>
       </c>
@@ -2071,7 +2107,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="24" customFormat="1">
+    <row r="34" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>299</v>
       </c>
@@ -2088,7 +2124,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="24" customFormat="1">
+    <row r="35" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>299</v>
       </c>
@@ -2105,7 +2141,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="24" customFormat="1">
+    <row r="36" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>299</v>
       </c>
@@ -2122,7 +2158,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="14" customFormat="1">
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>299</v>
       </c>
@@ -2139,7 +2175,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="14" customFormat="1">
+    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>299</v>
       </c>
@@ -2156,7 +2192,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1">
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>204</v>
@@ -2171,7 +2207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1">
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>117</v>
@@ -2186,7 +2222,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>25</v>
       </c>
@@ -2200,7 +2236,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42" s="2">
         <v>26</v>
       </c>
@@ -2214,7 +2250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2228,7 +2264,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2242,49 +2278,52 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="B45" s="2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3">
         <v>29</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="B46" s="2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3">
         <v>30</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="B47" s="2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3">
         <v>31</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
         <v>32</v>
       </c>
@@ -2298,7 +2337,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>16</v>
       </c>
@@ -2315,7 +2354,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2332,7 +2371,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>17</v>
       </c>
@@ -2349,7 +2388,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>17</v>
       </c>
@@ -2366,7 +2405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1">
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2383,7 +2422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="8" customFormat="1">
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2400,7 +2439,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="8" customFormat="1">
+    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2417,7 +2456,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1">
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>72</v>
       </c>
@@ -2434,7 +2473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="8" customFormat="1">
+    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2451,7 +2490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="8" customFormat="1">
+    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2468,7 +2507,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="8" customFormat="1">
+    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2485,7 +2524,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="8" customFormat="1">
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2502,7 +2541,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" s="2">
         <v>45</v>
       </c>
@@ -2516,7 +2555,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
         <v>46</v>
       </c>
@@ -2530,7 +2569,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="2">
         <v>47</v>
       </c>
@@ -2544,7 +2583,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" s="2">
         <v>48</v>
       </c>
@@ -2558,7 +2597,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="8" customFormat="1">
+    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>67</v>
       </c>
@@ -2575,7 +2614,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="8" customFormat="1">
+    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>68</v>
       </c>
@@ -2592,7 +2631,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="8" customFormat="1">
+    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>69</v>
       </c>
@@ -2609,7 +2648,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="8" customFormat="1">
+    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>73</v>
       </c>
@@ -2626,7 +2665,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="8" customFormat="1">
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>67</v>
       </c>
@@ -2643,7 +2682,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>67</v>
       </c>
@@ -2660,7 +2699,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1">
+    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>67</v>
       </c>
@@ -2677,7 +2716,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1">
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>67</v>
       </c>
@@ -2694,7 +2733,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1">
+    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>67</v>
       </c>
@@ -2711,7 +2750,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1">
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>67</v>
       </c>
@@ -2728,7 +2767,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1">
+    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>67</v>
       </c>
@@ -2745,7 +2784,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1">
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>67</v>
       </c>
@@ -2762,7 +2801,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="8" customFormat="1">
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>69</v>
       </c>
@@ -2779,7 +2818,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>69</v>
       </c>
@@ -2796,7 +2835,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>106</v>
       </c>
@@ -2813,7 +2852,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>106</v>
       </c>
@@ -2830,7 +2869,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>106</v>
       </c>
@@ -2847,7 +2886,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>106</v>
       </c>
@@ -2864,7 +2903,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>106</v>
       </c>
@@ -2881,7 +2920,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>106</v>
       </c>
@@ -2898,7 +2937,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1">
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12" t="s">
         <v>117</v>
       </c>
@@ -2915,7 +2954,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1">
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="s">
         <v>121</v>
       </c>
@@ -2932,7 +2971,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="8" customFormat="1">
+    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>123</v>
       </c>
@@ -2949,7 +2988,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="8" customFormat="1">
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>123</v>
       </c>
@@ -2966,7 +3005,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1">
+    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>123</v>
       </c>
@@ -2983,7 +3022,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1">
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>131</v>
       </c>
@@ -3000,7 +3039,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1">
+    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>131</v>
       </c>
@@ -3017,7 +3056,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1">
+    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>131</v>
       </c>
@@ -3034,7 +3073,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1">
+    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>131</v>
       </c>
@@ -3051,7 +3090,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1">
+    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>131</v>
       </c>
@@ -3068,7 +3107,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1">
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>131</v>
       </c>
@@ -3085,7 +3124,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1">
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>131</v>
       </c>
@@ -3102,7 +3141,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1">
+    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>131</v>
       </c>
@@ -3119,7 +3158,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1">
+    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>131</v>
       </c>
@@ -3136,7 +3175,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1">
+    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>131</v>
       </c>
@@ -3153,7 +3192,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1">
+    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>132</v>
       </c>
@@ -3170,7 +3209,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1">
+    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>132</v>
       </c>
@@ -3187,7 +3226,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1">
+    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>132</v>
       </c>
@@ -3204,7 +3243,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1">
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>132</v>
       </c>
@@ -3221,7 +3260,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1">
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>132</v>
       </c>
@@ -3238,7 +3277,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="4" customFormat="1">
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>132</v>
       </c>
@@ -3255,7 +3294,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1">
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>132</v>
       </c>
@@ -3272,7 +3311,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1">
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>132</v>
       </c>
@@ -3289,7 +3328,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1">
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>176</v>
       </c>
@@ -3306,7 +3345,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1">
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>176</v>
       </c>
@@ -3323,7 +3362,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1">
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>182</v>
       </c>
@@ -3340,7 +3379,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1">
+    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>183</v>
       </c>
@@ -3357,7 +3396,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1">
+    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>176</v>
       </c>
@@ -3374,7 +3413,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1">
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>117</v>
       </c>
@@ -3391,7 +3430,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1">
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>176</v>
       </c>
@@ -3408,7 +3447,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>191</v>
       </c>
@@ -3425,7 +3464,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1">
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>202</v>
       </c>
@@ -3442,7 +3481,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1">
+    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>123</v>
       </c>
@@ -3459,7 +3498,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1">
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>123</v>
       </c>
@@ -3476,7 +3515,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="8" customFormat="1">
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>183</v>
       </c>
@@ -3493,7 +3532,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="8" customFormat="1">
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>183</v>
       </c>
@@ -3510,7 +3549,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1">
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>183</v>
       </c>
@@ -3527,7 +3566,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1">
+    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>183</v>
       </c>
@@ -3544,7 +3583,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1">
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>73</v>
       </c>
@@ -3561,7 +3600,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="27" customFormat="1">
+    <row r="124" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="26" t="s">
         <v>176</v>
       </c>
@@ -3578,7 +3617,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="29" customFormat="1">
+    <row r="125" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="28"/>
       <c r="B125" s="28" t="s">
         <v>232</v>
@@ -3591,7 +3630,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1">
+    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
         <v>233</v>
@@ -3606,7 +3645,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1">
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>235</v>
@@ -3621,7 +3660,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1">
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
         <v>237</v>
@@ -3636,7 +3675,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1">
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
         <v>239</v>
@@ -3649,7 +3688,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1">
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>241</v>
@@ -3664,7 +3703,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="4" customFormat="1">
+    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
         <v>243</v>
@@ -3679,7 +3718,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1">
+    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>245</v>
@@ -3694,7 +3733,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="8" customFormat="1">
+    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
         <v>247</v>
@@ -3709,7 +3748,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1">
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>249</v>
@@ -3724,7 +3763,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="4" customFormat="1">
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>251</v>
@@ -3739,7 +3778,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="4" customFormat="1">
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>252</v>
@@ -3754,7 +3793,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B137" s="2" t="s">
         <v>254</v>
       </c>
@@ -3768,7 +3807,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B138" s="2" t="s">
         <v>256</v>
       </c>
@@ -3782,7 +3821,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B139" s="2" t="s">
         <v>258</v>
       </c>
@@ -3796,7 +3835,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B140" s="2" t="s">
         <v>260</v>
       </c>
@@ -3810,7 +3849,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B141" s="2" t="s">
         <v>262</v>
       </c>
@@ -3824,7 +3863,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B142" s="2" t="s">
         <v>264</v>
       </c>
@@ -3838,7 +3877,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B143" s="2" t="s">
         <v>267</v>
       </c>
@@ -3852,7 +3891,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B144" s="2" t="s">
         <v>270</v>
       </c>
@@ -3866,7 +3905,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="145" spans="2:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B145" s="2" t="s">
         <v>272</v>
       </c>
@@ -3880,7 +3919,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="146" spans="2:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B146" s="2" t="s">
         <v>274</v>
       </c>
@@ -3894,7 +3933,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="147" spans="2:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B147" s="2" t="s">
         <v>276</v>
       </c>
@@ -3908,7 +3947,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="148" spans="2:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B148" s="2" t="s">
         <v>278</v>
       </c>
@@ -3922,7 +3961,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="149" spans="2:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B149" s="2" t="s">
         <v>280</v>
       </c>
@@ -3936,7 +3975,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="150" spans="2:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B150" s="2" t="s">
         <v>282</v>
       </c>
@@ -3950,7 +3989,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="151" spans="2:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B151" s="2" t="s">
         <v>284</v>
       </c>
@@ -3961,7 +4000,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="152" spans="2:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B152" s="2" t="s">
         <v>286</v>
       </c>
@@ -3972,7 +4011,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="153" spans="2:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B153" s="2" t="s">
         <v>300</v>
       </c>
@@ -3986,7 +4025,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="154" spans="2:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B154" s="2" t="s">
         <v>302</v>
       </c>
@@ -3998,6 +4037,58 @@
       </c>
       <c r="E154" s="2" t="s">
         <v>303</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D155" s="3"/>
+      <c r="E155" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D156" s="3"/>
+      <c r="E156" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D157" s="3"/>
+      <c r="E157" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D158" s="3"/>
+      <c r="E158" s="4" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4007,24 +4098,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated requirements, add REQ ID's to basicSearch tests
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\Projects\MovieDbCode\MovieDb\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="9132"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="349">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -1373,6 +1368,30 @@
   </si>
   <si>
     <t>Controller that properly deletes a person, and all corresponding person information from the database (including album/images).</t>
+  </si>
+  <si>
+    <t>Searching for an empty string returns a comprehensive list of all movie and people results</t>
+  </si>
+  <si>
+    <t>When searching for a string, if any movie matches are found, then only the movie results are displayed.</t>
+  </si>
+  <si>
+    <t>When searching for a string, if no movie matches are found then any people matches are shown instead.</t>
+  </si>
+  <si>
+    <t>When searching for a string, if no movie or people matches are found, then display a comprehensive list of all movie and people results.</t>
+  </si>
+  <si>
+    <t>When searching for a string, a substring can be a match.</t>
+  </si>
+  <si>
+    <t>When searching for a string, if the string contains more than one word then individual words can be a match.</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1622,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1638,7 +1657,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1847,53 +1866,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171:D175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="208.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E4" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E5" s="9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E6" s="14" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -1910,7 +1929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>127</v>
       </c>
@@ -1927,7 +1946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>128</v>
       </c>
@@ -1944,7 +1963,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>129</v>
       </c>
@@ -1961,21 +1980,21 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -1989,7 +2008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -2003,7 +2022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -2017,7 +2036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3">
         <v>8</v>
@@ -2032,7 +2051,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3">
         <v>9</v>
@@ -2047,7 +2066,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -2061,7 +2080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -2075,7 +2094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -2089,7 +2108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -2103,7 +2122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -2117,7 +2136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -2131,7 +2150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>294</v>
       </c>
@@ -2148,7 +2167,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>294</v>
       </c>
@@ -2165,7 +2184,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>294</v>
       </c>
@@ -2182,7 +2201,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>294</v>
       </c>
@@ -2199,7 +2218,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>294</v>
       </c>
@@ -2216,7 +2235,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>294</v>
       </c>
@@ -2233,7 +2252,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
         <v>294</v>
       </c>
@@ -2250,7 +2269,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>294</v>
       </c>
@@ -2267,7 +2286,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>201</v>
@@ -2282,7 +2301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>114</v>
@@ -2297,7 +2316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>25</v>
       </c>
@@ -2311,7 +2330,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>26</v>
       </c>
@@ -2325,7 +2344,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2339,7 +2358,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2353,7 +2372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>29</v>
       </c>
@@ -2367,7 +2386,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>30</v>
       </c>
@@ -2381,7 +2400,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>31</v>
       </c>
@@ -2395,7 +2414,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
         <v>32</v>
       </c>
@@ -2409,7 +2428,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>16</v>
       </c>
@@ -2426,7 +2445,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2443,41 +2462,41 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+    <row r="51" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
         <v>17</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="9">
         <v>35</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+    <row r="52" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9">
         <v>17</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="9">
         <v>36</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2494,7 +2513,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2511,7 +2530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2528,7 +2547,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>69</v>
       </c>
@@ -2545,7 +2564,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2562,7 +2581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2579,7 +2598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2596,7 +2615,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2613,7 +2632,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B61" s="2">
         <v>45</v>
       </c>
@@ -2627,7 +2646,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B62" s="2">
         <v>46</v>
       </c>
@@ -2641,7 +2660,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B63" s="2">
         <v>47</v>
       </c>
@@ -2655,7 +2674,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B64" s="2">
         <v>48</v>
       </c>
@@ -2669,7 +2688,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>64</v>
       </c>
@@ -2686,7 +2705,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -2703,7 +2722,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>66</v>
       </c>
@@ -2720,7 +2739,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>70</v>
       </c>
@@ -2737,7 +2756,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>64</v>
       </c>
@@ -2754,7 +2773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>64</v>
       </c>
@@ -2771,7 +2790,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>64</v>
       </c>
@@ -2788,7 +2807,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>64</v>
       </c>
@@ -2805,7 +2824,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>64</v>
       </c>
@@ -2822,7 +2841,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>64</v>
       </c>
@@ -2839,7 +2858,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>64</v>
       </c>
@@ -2856,7 +2875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>64</v>
       </c>
@@ -2873,7 +2892,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>66</v>
       </c>
@@ -2890,7 +2909,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>66</v>
       </c>
@@ -2907,7 +2926,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>103</v>
       </c>
@@ -2924,7 +2943,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
@@ -2941,7 +2960,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>103</v>
       </c>
@@ -2958,7 +2977,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>103</v>
       </c>
@@ -2975,7 +2994,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>103</v>
       </c>
@@ -2992,7 +3011,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>103</v>
       </c>
@@ -3009,7 +3028,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
         <v>114</v>
       </c>
@@ -3026,7 +3045,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
         <v>118</v>
       </c>
@@ -3043,7 +3062,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>120</v>
       </c>
@@ -3060,7 +3079,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>120</v>
       </c>
@@ -3077,7 +3096,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>120</v>
       </c>
@@ -3094,7 +3113,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>128</v>
       </c>
@@ -3111,7 +3130,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>128</v>
       </c>
@@ -3128,7 +3147,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>128</v>
       </c>
@@ -3145,7 +3164,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>128</v>
       </c>
@@ -3162,7 +3181,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>128</v>
       </c>
@@ -3179,7 +3198,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>128</v>
       </c>
@@ -3196,7 +3215,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>128</v>
       </c>
@@ -3213,7 +3232,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>128</v>
       </c>
@@ -3230,7 +3249,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>128</v>
       </c>
@@ -3247,7 +3266,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>128</v>
       </c>
@@ -3264,7 +3283,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>129</v>
       </c>
@@ -3281,7 +3300,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>129</v>
       </c>
@@ -3298,7 +3317,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>129</v>
       </c>
@@ -3315,7 +3334,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>129</v>
       </c>
@@ -3332,7 +3351,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>129</v>
       </c>
@@ -3349,7 +3368,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>129</v>
       </c>
@@ -3366,7 +3385,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>129</v>
       </c>
@@ -3383,7 +3402,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>129</v>
       </c>
@@ -3400,7 +3419,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>173</v>
       </c>
@@ -3417,7 +3436,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>173</v>
       </c>
@@ -3434,7 +3453,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>179</v>
       </c>
@@ -3451,7 +3470,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>180</v>
       </c>
@@ -3468,7 +3487,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>173</v>
       </c>
@@ -3485,7 +3504,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>114</v>
       </c>
@@ -3502,7 +3521,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>173</v>
       </c>
@@ -3519,7 +3538,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>188</v>
       </c>
@@ -3536,7 +3555,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>199</v>
       </c>
@@ -3553,7 +3572,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>120</v>
       </c>
@@ -3570,7 +3589,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>120</v>
       </c>
@@ -3587,7 +3606,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>180</v>
       </c>
@@ -3604,7 +3623,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>180</v>
       </c>
@@ -3621,7 +3640,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>180</v>
       </c>
@@ -3638,7 +3657,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>180</v>
       </c>
@@ -3655,7 +3674,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>70</v>
       </c>
@@ -3672,7 +3691,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="23" t="s">
         <v>173</v>
       </c>
@@ -3689,7 +3708,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="25"/>
       <c r="B125" s="25" t="s">
         <v>229</v>
@@ -3702,7 +3721,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
         <v>230</v>
@@ -3717,7 +3736,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>232</v>
@@ -3732,7 +3751,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
         <v>234</v>
@@ -3747,7 +3766,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
         <v>236</v>
@@ -3760,7 +3779,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>238</v>
@@ -3775,7 +3794,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
         <v>240</v>
@@ -3790,7 +3809,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>242</v>
@@ -3805,7 +3824,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
         <v>244</v>
@@ -3820,7 +3839,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>246</v>
@@ -3835,7 +3854,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>248</v>
@@ -3850,7 +3869,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>249</v>
@@ -3865,7 +3884,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
         <v>251</v>
@@ -3880,7 +3899,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
         <v>253</v>
@@ -3895,7 +3914,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
         <v>255</v>
@@ -3910,7 +3929,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="B140" s="3" t="s">
         <v>257</v>
@@ -3925,7 +3944,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3"/>
       <c r="B141" s="3" t="s">
         <v>259</v>
@@ -3940,7 +3959,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
         <v>261</v>
@@ -3955,7 +3974,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3"/>
       <c r="B143" s="3" t="s">
         <v>264</v>
@@ -3970,7 +3989,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3"/>
       <c r="B144" s="3" t="s">
         <v>267</v>
@@ -3985,7 +4004,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
         <v>269</v>
@@ -4000,7 +4019,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
         <v>271</v>
@@ -4015,7 +4034,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
         <v>273</v>
@@ -4030,7 +4049,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
         <v>275</v>
@@ -4045,7 +4064,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3"/>
       <c r="B149" s="3" t="s">
         <v>277</v>
@@ -4060,7 +4079,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3"/>
       <c r="B150" s="3" t="s">
         <v>279</v>
@@ -4075,7 +4094,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
         <v>281</v>
@@ -4088,7 +4107,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
         <v>283</v>
@@ -4101,7 +4120,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
         <v>295</v>
@@ -4116,7 +4135,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
         <v>297</v>
@@ -4131,7 +4150,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3"/>
       <c r="B155" s="3" t="s">
         <v>301</v>
@@ -4144,7 +4163,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3"/>
       <c r="B156" s="3" t="s">
         <v>303</v>
@@ -4159,7 +4178,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3"/>
       <c r="B157" s="3" t="s">
         <v>304</v>
@@ -4174,7 +4193,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3"/>
       <c r="B158" s="3" t="s">
         <v>306</v>
@@ -4189,7 +4208,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3"/>
       <c r="B159" s="3" t="s">
         <v>310</v>
@@ -4204,7 +4223,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3"/>
       <c r="B160" s="3" t="s">
         <v>311</v>
@@ -4217,7 +4236,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3"/>
       <c r="B161" s="3" t="s">
         <v>313</v>
@@ -4230,7 +4249,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B162" s="2" t="s">
         <v>315</v>
       </c>
@@ -4241,7 +4260,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B163" s="2" t="s">
         <v>316</v>
       </c>
@@ -4252,7 +4271,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3"/>
       <c r="B164" s="3" t="s">
         <v>318</v>
@@ -4265,7 +4284,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3"/>
       <c r="B165" s="3" t="s">
         <v>320</v>
@@ -4280,7 +4299,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3"/>
       <c r="B166" s="3" t="s">
         <v>324</v>
@@ -4295,7 +4314,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3"/>
       <c r="B167" s="3" t="s">
         <v>326</v>
@@ -4310,7 +4329,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3"/>
       <c r="B168" s="3" t="s">
         <v>328</v>
@@ -4323,7 +4342,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B169" s="2" t="s">
         <v>330</v>
       </c>
@@ -4334,7 +4353,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3"/>
       <c r="B170" s="3" t="s">
         <v>335</v>
@@ -4347,6 +4366,90 @@
       </c>
       <c r="E170" s="3" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="3">
+        <v>155</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D171" s="3">
+        <v>4</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="3">
+        <v>156</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D172" s="3">
+        <v>4</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B173" s="3">
+        <v>157</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D173" s="3">
+        <v>4</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="3">
+        <v>158</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D174" s="3">
+        <v>4</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="3">
+        <v>159</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" s="3">
+        <v>4</v>
+      </c>
+      <c r="E175" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B176" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E176" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -4361,7 +4464,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4373,7 +4476,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated commit , funct. reqs.
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytonjohnson/Desktop/Projects/MovieDbCode/MovieDb/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="9132"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="357">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -1392,6 +1402,30 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>The post a reply button should redirect user to Reply creation page.</t>
+  </si>
+  <si>
+    <t>Navigating to ./discussions/create/{mid} should take user to discussion creation page.</t>
+  </si>
+  <si>
+    <t>Discussion creation form should be properly saved to the database.</t>
+  </si>
+  <si>
+    <t>Most recent discussions should appear on landing page.</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
   </si>
 </sst>
 </file>
@@ -1622,12 +1656,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1657,12 +1691,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1866,53 +1900,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E176"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171:D175"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="208.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="208.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E6" s="14" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -1929,7 +1963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>127</v>
       </c>
@@ -1946,7 +1980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>128</v>
       </c>
@@ -1963,7 +1997,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>129</v>
       </c>
@@ -1980,7 +2014,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>4</v>
       </c>
@@ -1994,7 +2028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -2008,7 +2042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -2022,7 +2056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -2036,7 +2070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3">
         <v>8</v>
@@ -2051,7 +2085,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3">
         <v>9</v>
@@ -2066,7 +2100,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -2080,7 +2114,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>11</v>
       </c>
@@ -2094,7 +2128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>12</v>
       </c>
@@ -2108,7 +2142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>13</v>
       </c>
@@ -2122,7 +2156,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>14</v>
       </c>
@@ -2136,7 +2170,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>15</v>
       </c>
@@ -2150,7 +2184,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>294</v>
       </c>
@@ -2167,7 +2201,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>294</v>
       </c>
@@ -2184,7 +2218,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>294</v>
       </c>
@@ -2201,7 +2235,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>294</v>
       </c>
@@ -2218,7 +2252,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
         <v>294</v>
       </c>
@@ -2235,7 +2269,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
         <v>294</v>
       </c>
@@ -2252,7 +2286,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>294</v>
       </c>
@@ -2269,7 +2303,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>294</v>
       </c>
@@ -2286,7 +2320,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
         <v>201</v>
@@ -2301,7 +2335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
         <v>114</v>
@@ -2316,7 +2350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>25</v>
       </c>
@@ -2330,7 +2364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42" s="2">
         <v>26</v>
       </c>
@@ -2344,7 +2378,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -2358,7 +2392,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -2372,49 +2406,52 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3">
         <v>29</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3">
         <v>30</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3">
         <v>31</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
         <v>32</v>
       </c>
@@ -2428,7 +2465,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>16</v>
       </c>
@@ -2445,7 +2482,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>17</v>
       </c>
@@ -2462,7 +2499,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>17</v>
       </c>
@@ -2479,7 +2516,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
         <v>17</v>
       </c>
@@ -2496,7 +2533,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>6</v>
       </c>
@@ -2513,7 +2550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>3</v>
       </c>
@@ -2530,7 +2567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>5</v>
       </c>
@@ -2547,7 +2584,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>69</v>
       </c>
@@ -2564,7 +2601,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>10</v>
       </c>
@@ -2581,7 +2618,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>18</v>
       </c>
@@ -2598,7 +2635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2615,7 +2652,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>6</v>
       </c>
@@ -2632,7 +2669,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" s="2">
         <v>45</v>
       </c>
@@ -2646,7 +2683,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" s="2">
         <v>46</v>
       </c>
@@ -2660,7 +2697,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="2">
         <v>47</v>
       </c>
@@ -2674,7 +2711,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" s="2">
         <v>48</v>
       </c>
@@ -2688,7 +2725,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>64</v>
       </c>
@@ -2705,7 +2742,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -2722,7 +2759,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>66</v>
       </c>
@@ -2739,7 +2776,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>70</v>
       </c>
@@ -2756,7 +2793,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>64</v>
       </c>
@@ -2773,7 +2810,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>64</v>
       </c>
@@ -2790,7 +2827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>64</v>
       </c>
@@ -2807,7 +2844,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>64</v>
       </c>
@@ -2824,7 +2861,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>64</v>
       </c>
@@ -2841,7 +2878,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>64</v>
       </c>
@@ -2858,7 +2895,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>64</v>
       </c>
@@ -2875,7 +2912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>64</v>
       </c>
@@ -2892,7 +2929,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>66</v>
       </c>
@@ -2909,7 +2946,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>66</v>
       </c>
@@ -2926,7 +2963,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>103</v>
       </c>
@@ -2943,7 +2980,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
@@ -2960,7 +2997,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>103</v>
       </c>
@@ -2977,7 +3014,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>103</v>
       </c>
@@ -2994,7 +3031,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>103</v>
       </c>
@@ -3011,7 +3048,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>103</v>
       </c>
@@ -3028,7 +3065,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12" t="s">
         <v>114</v>
       </c>
@@ -3045,7 +3082,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="s">
         <v>118</v>
       </c>
@@ -3062,7 +3099,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>120</v>
       </c>
@@ -3079,7 +3116,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>120</v>
       </c>
@@ -3096,7 +3133,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>120</v>
       </c>
@@ -3113,7 +3150,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>128</v>
       </c>
@@ -3130,7 +3167,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>128</v>
       </c>
@@ -3147,7 +3184,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>128</v>
       </c>
@@ -3164,7 +3201,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>128</v>
       </c>
@@ -3181,7 +3218,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>128</v>
       </c>
@@ -3198,7 +3235,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>128</v>
       </c>
@@ -3215,7 +3252,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>128</v>
       </c>
@@ -3232,7 +3269,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>128</v>
       </c>
@@ -3249,7 +3286,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>128</v>
       </c>
@@ -3266,7 +3303,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>128</v>
       </c>
@@ -3283,7 +3320,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>129</v>
       </c>
@@ -3300,7 +3337,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>129</v>
       </c>
@@ -3317,7 +3354,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>129</v>
       </c>
@@ -3334,7 +3371,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>129</v>
       </c>
@@ -3351,7 +3388,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>129</v>
       </c>
@@ -3368,7 +3405,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>129</v>
       </c>
@@ -3385,7 +3422,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>129</v>
       </c>
@@ -3402,7 +3439,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>129</v>
       </c>
@@ -3419,7 +3456,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>173</v>
       </c>
@@ -3436,7 +3473,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>173</v>
       </c>
@@ -3453,7 +3490,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>179</v>
       </c>
@@ -3470,7 +3507,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>180</v>
       </c>
@@ -3487,7 +3524,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>173</v>
       </c>
@@ -3504,7 +3541,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>114</v>
       </c>
@@ -3521,7 +3558,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>173</v>
       </c>
@@ -3538,7 +3575,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>188</v>
       </c>
@@ -3555,7 +3592,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>199</v>
       </c>
@@ -3572,7 +3609,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>120</v>
       </c>
@@ -3589,7 +3626,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>120</v>
       </c>
@@ -3606,7 +3643,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>180</v>
       </c>
@@ -3623,7 +3660,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>180</v>
       </c>
@@ -3640,7 +3677,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>180</v>
       </c>
@@ -3657,7 +3694,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>180</v>
       </c>
@@ -3674,7 +3711,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>70</v>
       </c>
@@ -3691,7 +3728,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23" t="s">
         <v>173</v>
       </c>
@@ -3708,7 +3745,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="25"/>
       <c r="B125" s="25" t="s">
         <v>229</v>
@@ -3721,7 +3758,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
         <v>230</v>
@@ -3736,7 +3773,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
         <v>232</v>
@@ -3751,7 +3788,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
         <v>234</v>
@@ -3766,7 +3803,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
         <v>236</v>
@@ -3779,7 +3816,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
         <v>238</v>
@@ -3794,7 +3831,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
         <v>240</v>
@@ -3809,7 +3846,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
         <v>242</v>
@@ -3824,7 +3861,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
         <v>244</v>
@@ -3839,7 +3876,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
         <v>246</v>
@@ -3854,7 +3891,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
         <v>248</v>
@@ -3869,7 +3906,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
         <v>249</v>
@@ -3884,7 +3921,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
         <v>251</v>
@@ -3899,7 +3936,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
         <v>253</v>
@@ -3914,7 +3951,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
         <v>255</v>
@@ -3929,7 +3966,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3"/>
       <c r="B140" s="3" t="s">
         <v>257</v>
@@ -3944,7 +3981,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3"/>
       <c r="B141" s="3" t="s">
         <v>259</v>
@@ -3959,7 +3996,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
         <v>261</v>
@@ -3974,7 +4011,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3"/>
       <c r="B143" s="3" t="s">
         <v>264</v>
@@ -3989,7 +4026,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3"/>
       <c r="B144" s="3" t="s">
         <v>267</v>
@@ -4004,7 +4041,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
         <v>269</v>
@@ -4019,7 +4056,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
         <v>271</v>
@@ -4034,7 +4071,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
         <v>273</v>
@@ -4049,7 +4086,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
         <v>275</v>
@@ -4064,7 +4101,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3"/>
       <c r="B149" s="3" t="s">
         <v>277</v>
@@ -4079,7 +4116,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="3" t="s">
         <v>279</v>
@@ -4094,7 +4131,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
         <v>281</v>
@@ -4107,7 +4144,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
         <v>283</v>
@@ -4120,7 +4157,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
         <v>295</v>
@@ -4135,7 +4172,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
         <v>297</v>
@@ -4150,7 +4187,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="3" t="s">
         <v>301</v>
@@ -4163,7 +4200,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
       <c r="B156" s="3" t="s">
         <v>303</v>
@@ -4178,7 +4215,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
       <c r="B157" s="3" t="s">
         <v>304</v>
@@ -4193,7 +4230,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
       <c r="B158" s="3" t="s">
         <v>306</v>
@@ -4208,7 +4245,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
       <c r="B159" s="3" t="s">
         <v>310</v>
@@ -4223,7 +4260,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3"/>
       <c r="B160" s="3" t="s">
         <v>311</v>
@@ -4236,7 +4273,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
       <c r="B161" s="3" t="s">
         <v>313</v>
@@ -4249,7 +4286,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B162" s="2" t="s">
         <v>315</v>
       </c>
@@ -4260,7 +4297,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B163" s="2" t="s">
         <v>316</v>
       </c>
@@ -4271,7 +4308,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
       <c r="B164" s="3" t="s">
         <v>318</v>
@@ -4284,7 +4321,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="3" t="s">
         <v>320</v>
@@ -4299,7 +4336,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
       <c r="B166" s="3" t="s">
         <v>324</v>
@@ -4314,7 +4351,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
       <c r="B167" s="3" t="s">
         <v>326</v>
@@ -4329,7 +4366,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3"/>
       <c r="B168" s="3" t="s">
         <v>328</v>
@@ -4342,7 +4379,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B169" s="2" t="s">
         <v>330</v>
       </c>
@@ -4353,7 +4390,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3"/>
       <c r="B170" s="3" t="s">
         <v>335</v>
@@ -4368,7 +4405,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B171" s="3">
         <v>155</v>
       </c>
@@ -4382,7 +4419,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B172" s="3">
         <v>156</v>
       </c>
@@ -4396,7 +4433,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B173" s="3">
         <v>157</v>
       </c>
@@ -4410,7 +4447,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B174" s="3">
         <v>158</v>
       </c>
@@ -4424,7 +4461,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B175" s="3">
         <v>159</v>
       </c>
@@ -4438,7 +4475,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B176" s="2" t="s">
         <v>347</v>
       </c>
@@ -4450,6 +4487,58 @@
       </c>
       <c r="E176" t="s">
         <v>346</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" s="3"/>
+      <c r="B177" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D177" s="3"/>
+      <c r="E177" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" s="3"/>
+      <c r="B178" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D178" s="3"/>
+      <c r="E178" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D179" s="3"/>
+      <c r="E179" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" s="3"/>
+      <c r="B180" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D180" s="3"/>
+      <c r="E180" s="4" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4464,7 +4553,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4476,7 +4565,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Assigning test IDs to tests
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claytonjohnson/Desktop/Projects/MovieDbCode/MovieDb/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23265" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="362">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -62,9 +57,6 @@
   </si>
   <si>
     <t>A View and Controller where you can fill in a form regarding user information required. Firstname, Lastname, Username, Password, Email. Form is validated through JS.</t>
-  </si>
-  <si>
-    <t>View and Controller for log-in page. Usernamd and Password. Validation through JS. User is redirected to user page.</t>
   </si>
   <si>
     <t>Movie Page</t>
@@ -1209,9 +1201,6 @@
     <t>136</t>
   </si>
   <si>
-    <t>TESTING IN PROGRESS</t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -1371,9 +1360,6 @@
     <t>The pictures section of a movie page contains a button "view all pictures" that redirects a person to an album preview page.</t>
   </si>
   <si>
-    <t>If a user attempts to display a review that does not exist, a review not found page is displayed.</t>
-  </si>
-  <si>
     <t>Controller that properly deletes a movie, and all corresponding movie information from the database (includes reviews, discussions and album/images).</t>
   </si>
   <si>
@@ -1426,6 +1412,30 @@
   </si>
   <si>
     <t>164</t>
+  </si>
+  <si>
+    <t>UNIMPLEMENTED</t>
+  </si>
+  <si>
+    <t>Users have roles, which define the class of that user for the site.</t>
+  </si>
+  <si>
+    <t>View and Controller for log-in page. Username and Password. Validation through JS. User is redirected to user page.</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>Roles have permissions, which define the actions that a role can perform on the site.</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>IMPLEMENTED &amp; UNTESTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1525,28 +1535,25 @@
         <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF5F5F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1555,7 +1562,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1572,19 +1579,25 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1595,6 +1608,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEF5F5F"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFFFFF99"/>
@@ -1656,7 +1670,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1691,7 +1705,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1900,55 +1914,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="E184" sqref="E184"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="208.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="208.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C1" s="5"/>
       <c r="E1" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E6" s="14" t="s">
-        <v>284</v>
+      <c r="E6" s="21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="22" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>0</v>
@@ -1965,7 +1984,7 @@
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -1982,7 +2001,7 @@
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1991,15 +2010,15 @@
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -2008,10 +2027,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2067,7 +2086,7 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2076,13 +2095,13 @@
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2091,13 +2110,13 @@
         <v>9</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2105,13 +2124,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
         <v>16</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2119,13 +2138,13 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="2">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2133,13 +2152,13 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="2">
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2147,13 +2166,13 @@
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="2">
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2161,13 +2180,13 @@
         <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="2">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2175,155 +2194,155 @@
         <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="2">
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
-        <v>294</v>
-      </c>
-      <c r="B31" s="17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="B31" s="29">
         <v>16</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="17" t="s">
+      <c r="C31" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="30" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="16">
+        <v>17</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B33" s="16">
+        <v>18</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B35" s="16">
+        <v>19</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B32" s="20">
-        <v>17</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="22" t="s">
+    <row r="36" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B36" s="16">
+        <v>20</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B33" s="20">
-        <v>18</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>293</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="22" t="s">
+    <row r="37" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B35" s="20">
-        <v>19</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B36" s="20">
-        <v>20</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B37" s="20">
+      <c r="B37" s="16">
         <v>21</v>
       </c>
-      <c r="C37" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="B38" s="20">
+      <c r="C37" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B38" s="16">
         <v>22</v>
       </c>
-      <c r="C38" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>340</v>
+      <c r="C38" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>4</v>
@@ -2332,13 +2351,13 @@
         <v>6</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>4</v>
@@ -2347,21 +2366,22 @@
         <v>6</v>
       </c>
       <c r="E40" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10">
+        <v>25</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="2">
-        <v>25</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" s="10">
+        <v>6</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D41" s="2">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2369,41 +2389,41 @@
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2412,13 +2432,13 @@
         <v>29</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2427,13 +2447,13 @@
         <v>30</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2442,44 +2462,45 @@
         <v>31</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="24"/>
+      <c r="B48" s="24">
+        <v>32</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="24">
+        <v>6</v>
+      </c>
+      <c r="E48" s="22" t="s">
         <v>38</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="2">
-        <v>32</v>
-      </c>
-      <c r="C48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="2">
-        <v>6</v>
-      </c>
-      <c r="E48" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>16</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="14">
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2496,41 +2517,41 @@
         <v>6</v>
       </c>
       <c r="E50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="23">
+        <v>17</v>
+      </c>
+      <c r="B51" s="23">
+        <v>35</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="9">
+    <row r="52" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23">
         <v>17</v>
       </c>
-      <c r="B51" s="9">
-        <v>35</v>
-      </c>
-      <c r="C51" s="9" t="s">
+      <c r="B52" s="23">
+        <v>36</v>
+      </c>
+      <c r="C52" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D52" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E52" s="22" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="9">
-        <v>17</v>
-      </c>
-      <c r="B52" s="9">
-        <v>36</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2541,13 +2562,13 @@
         <v>37</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2558,13 +2579,13 @@
         <v>38</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2575,30 +2596,30 @@
         <v>39</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B56" s="7">
         <v>40</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2609,13 +2630,13 @@
         <v>41</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D57" s="7">
         <v>40</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2626,13 +2647,13 @@
         <v>42</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2643,13 +2664,13 @@
         <v>43</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -2660,13 +2681,13 @@
         <v>44</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D60" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2674,13 +2695,13 @@
         <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2688,13 +2709,13 @@
         <v>46</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2702,13 +2723,13 @@
         <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2716,786 +2737,786 @@
         <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" s="7">
         <v>49</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" s="7">
         <v>50</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="7">
         <v>51</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D67" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="C68" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D68" s="7" t="s">
+      <c r="E68" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B69" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D69" s="7" t="s">
+      <c r="E69" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E69" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C70" t="s">
-        <v>62</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="25" t="s">
         <v>77</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D75" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="D77" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="E77" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="E78" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C80" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E80" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C81" t="s">
-        <v>57</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E81" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C82" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C82" t="s">
-        <v>57</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E82" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C84" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C84" t="s">
-        <v>57</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="C85" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E85" s="12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E86" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="B86" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="C87" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="109" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="110" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>4</v>
@@ -3504,15 +3525,15 @@
         <v>6</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="111" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>4</v>
@@ -3521,134 +3542,134 @@
         <v>6</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="C115" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B116" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B116" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="C116" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D116" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D117" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D118" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C118" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="D118" s="3" t="s">
+      <c r="E118" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>4</v>
@@ -3657,15 +3678,15 @@
         <v>6</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>4</v>
@@ -3674,735 +3695,739 @@
         <v>6</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="121" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D122" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C123" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D123" s="3" t="s">
+      <c r="E123" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E123" s="3" t="s">
+    </row>
+    <row r="124" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B124" s="19" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="23" t="s">
+      <c r="C124" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="B124" s="23" t="s">
+      <c r="E124" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="C124" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D124" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="E124" s="23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="25"/>
-      <c r="B125" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="C125" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D125" s="25"/>
-      <c r="E125" s="26" t="s">
-        <v>299</v>
+    </row>
+    <row r="125" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="26"/>
+      <c r="B125" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C125" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D125" s="26"/>
+      <c r="E125" s="27" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="126" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="B126" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E126" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="127" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3"/>
       <c r="B127" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E127" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="128" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
       <c r="B128" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E128" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E128" s="4" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="129" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
       <c r="B129" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
       <c r="B130" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E130" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E130" s="4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="131" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3"/>
       <c r="B131" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E131" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E131" s="4" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3"/>
       <c r="B132" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E132" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E132" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7"/>
       <c r="B133" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E133" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="C133" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D133" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3"/>
       <c r="B134" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E134" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E134" s="4" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="135" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="136" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3"/>
       <c r="B136" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E136" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E136" s="4" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="137" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3"/>
       <c r="B137" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E137" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E137" s="4" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="138" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3"/>
       <c r="B138" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E138" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E138" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="139" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3"/>
       <c r="B139" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E139" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E139" s="4" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="140" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3"/>
       <c r="B140" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E140" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E140" s="4" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="141" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3"/>
       <c r="B141" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E141" s="4" t="s">
         <v>259</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E141" s="4" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="142" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3"/>
       <c r="B142" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C142" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D142" s="3" t="s">
+      <c r="E142" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3"/>
       <c r="B143" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C143" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D143" s="3" t="s">
+      <c r="E143" s="4" t="s">
         <v>265</v>
-      </c>
-      <c r="E143" s="4" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3"/>
       <c r="B144" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E144" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="C144" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="E144" s="4" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="145" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3"/>
       <c r="B145" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E145" s="4" t="s">
         <v>269</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D145" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3"/>
       <c r="B146" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E146" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="C146" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D146" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E146" s="4" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="147" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3"/>
       <c r="B147" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E147" s="4" t="s">
         <v>273</v>
-      </c>
-      <c r="C147" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E147" s="4" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="148" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3"/>
       <c r="B148" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E148" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="C148" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E148" s="4" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="149" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3"/>
       <c r="B149" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E149" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E149" s="4" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="150" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3"/>
       <c r="B150" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E150" s="4" t="s">
         <v>279</v>
-      </c>
-      <c r="C150" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D150" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D151" s="3"/>
       <c r="E151" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D152" s="3"/>
       <c r="E152" s="4" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
     </row>
     <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="155" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D155" s="3"/>
       <c r="E155" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="156" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3"/>
       <c r="B156" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E156" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="157" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3"/>
       <c r="B157" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3"/>
       <c r="B158" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3"/>
       <c r="B159" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3"/>
       <c r="B160" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D160" s="3"/>
       <c r="E160" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3"/>
       <c r="B161" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D161" s="3"/>
       <c r="E161" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="3"/>
+      <c r="B162" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D162" s="3"/>
+      <c r="E162" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="3"/>
+      <c r="B163" s="3" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B162" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C162" t="s">
-        <v>302</v>
-      </c>
-      <c r="E162" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B163" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C163" t="s">
-        <v>302</v>
-      </c>
-      <c r="E163" t="s">
-        <v>331</v>
+      <c r="C163" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D163" s="3"/>
+      <c r="E163" s="4" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="164" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
       <c r="B164" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D164" s="3"/>
       <c r="E164" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="165" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
       <c r="B166" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3"/>
       <c r="B167" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3"/>
       <c r="B168" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D168" s="3"/>
       <c r="E168" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B169" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C169" t="s">
+        <v>197</v>
+      </c>
+      <c r="E169" t="s">
         <v>330</v>
-      </c>
-      <c r="C169" t="s">
-        <v>198</v>
-      </c>
-      <c r="E169" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3"/>
       <c r="B170" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="171" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4416,7 +4441,7 @@
         <v>4</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="172" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4430,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="173" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4444,7 +4469,7 @@
         <v>4</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="174" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4458,7 +4483,7 @@
         <v>4</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="175" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4472,73 +4497,103 @@
         <v>4</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B176" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E176" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="3"/>
       <c r="B177" s="3" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D177" s="3"/>
       <c r="E177" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="3"/>
       <c r="B178" s="3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D178" s="3"/>
       <c r="E178" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="3"/>
       <c r="B179" s="3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D179" s="3"/>
       <c r="E179" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="3"/>
       <c r="B180" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D180" s="3"/>
       <c r="E180" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="25"/>
+      <c r="B182" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="C182" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D182" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="E182" s="21" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -4553,7 +4608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4565,7 +4620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Description for REQ-ID 136 got deleted; Re-added
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -12,11 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1435,7 +1430,7 @@
     <t>IMPLEMENTED &amp; UNTESTED</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>If a user attempts to display a review that does no exist, a review not found page is displayed.</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1557,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1598,6 +1593,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1608,8 +1604,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
       <color rgb="FFEF5F5F"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFCC66FF"/>
@@ -1619,9 +1615,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1916,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="D136" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4152,7 +4145,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3" t="s">
         <v>280</v>
@@ -4165,7 +4158,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3" t="s">
         <v>282</v>
@@ -4174,11 +4167,11 @@
         <v>14</v>
       </c>
       <c r="D152" s="3"/>
-      <c r="E152" s="4" t="s">
+      <c r="E152" s="31" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3" t="s">
         <v>293</v>
@@ -4193,7 +4186,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3" t="s">
         <v>295</v>
@@ -4391,7 +4384,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="3" t="s">
         <v>326</v>
@@ -4404,7 +4397,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
         <v>328</v>
       </c>
@@ -4415,7 +4408,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="3" t="s">
         <v>333</v>
@@ -4430,7 +4423,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B171" s="3">
         <v>155</v>
       </c>
@@ -4444,7 +4437,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B172" s="3">
         <v>156</v>
       </c>
@@ -4458,7 +4451,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B173" s="3">
         <v>157</v>
       </c>
@@ -4472,7 +4465,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="3">
         <v>158</v>
       </c>
@@ -4486,7 +4479,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B175" s="3">
         <v>159</v>
       </c>
@@ -4500,7 +4493,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B176" s="2" t="s">
         <v>344</v>
       </c>
@@ -4514,7 +4507,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="3" t="s">
         <v>350</v>
@@ -4527,7 +4520,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="3" t="s">
         <v>351</v>
@@ -4540,7 +4533,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="3" t="s">
         <v>352</v>
@@ -4553,7 +4546,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="3" t="s">
         <v>353</v>

</xml_diff>

<commit_message>
Updating funtional requirements color codes
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="409">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -1485,6 +1485,93 @@
   </si>
   <si>
     <t>Clay/Tim</t>
+  </si>
+  <si>
+    <t>Be able to log in the website directly from the landing page</t>
+  </si>
+  <si>
+    <t>Checking the "remember me" saves the user's credentials for login</t>
+  </si>
+  <si>
+    <t>Clicking the forgot password button take the user to a page to recover their password</t>
+  </si>
+  <si>
+    <t>6, 33</t>
+  </si>
+  <si>
+    <t>Be able to register an account directly on the landing page</t>
+  </si>
+  <si>
+    <t>33, 8</t>
+  </si>
+  <si>
+    <t>Provide a list of the top 10 movies of the month</t>
+  </si>
+  <si>
+    <t>Provide clickable links to the movie pages in the top 10 movies of the month list</t>
+  </si>
+  <si>
+    <t>Provide a list of the top 10 recently released movies</t>
+  </si>
+  <si>
+    <t>33,8</t>
+  </si>
+  <si>
+    <t>Provide clickable links to the movie pages in the recently released movie list</t>
+  </si>
+  <si>
+    <t>33, 109</t>
+  </si>
+  <si>
+    <t>Provide a list of 3 recently added reviews to any movie</t>
+  </si>
+  <si>
+    <t>Allow user to click "see full review" to be taken to that review's page</t>
+  </si>
+  <si>
+    <t>If a user is logged in, the login and register boxes are not to be displayed</t>
+  </si>
+  <si>
+    <t>Provide a navigation bar, with search, advanced search, and links to the home page, user page, login and register pages</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>TIm</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1698,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1656,6 +1743,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1666,8 +1760,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
       <color rgb="FFEF5F5F"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFCC66FF"/>
@@ -1969,10 +2063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4807,35 +4901,35 @@
         <v>311</v>
       </c>
     </row>
-    <row r="162" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="2"/>
-      <c r="B162" s="2" t="s">
+    <row r="162" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="40"/>
+      <c r="B162" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C162" s="3" t="s">
+      <c r="C162" s="46" t="s">
         <v>299</v>
       </c>
-      <c r="D162" s="2"/>
-      <c r="E162" s="3" t="s">
+      <c r="D162" s="40"/>
+      <c r="E162" s="46" t="s">
         <v>377</v>
       </c>
-      <c r="F162" s="3" t="s">
+      <c r="F162" s="46" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="163" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="2"/>
-      <c r="B163" s="2" t="s">
+    <row r="163" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="40"/>
+      <c r="B163" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="C163" s="3" t="s">
+      <c r="C163" s="46" t="s">
         <v>299</v>
       </c>
-      <c r="D163" s="2"/>
-      <c r="E163" s="3" t="s">
+      <c r="D163" s="40"/>
+      <c r="E163" s="46" t="s">
         <v>378</v>
       </c>
-      <c r="F163" s="3" t="s">
+      <c r="F163" s="46" t="s">
         <v>328</v>
       </c>
     </row>
@@ -5175,6 +5269,215 @@
       </c>
       <c r="F183" s="37" t="s">
         <v>363</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="43"/>
+      <c r="B184" s="43" t="s">
+        <v>396</v>
+      </c>
+      <c r="C184" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D184" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="F184" s="44" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B185" s="42" t="s">
+        <v>397</v>
+      </c>
+      <c r="C185" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D185" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E185" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="F185" s="41" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B186" s="42" t="s">
+        <v>398</v>
+      </c>
+      <c r="C186" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D186" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E186" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="F186" s="41" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="43"/>
+      <c r="B187" s="43" t="s">
+        <v>399</v>
+      </c>
+      <c r="C187" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D187" s="43" t="s">
+        <v>383</v>
+      </c>
+      <c r="E187" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="F187" s="44" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B188" s="42" t="s">
+        <v>400</v>
+      </c>
+      <c r="C188" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D188" s="42" t="s">
+        <v>385</v>
+      </c>
+      <c r="E188" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="F188" s="41" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="43"/>
+      <c r="B189" s="43" t="s">
+        <v>401</v>
+      </c>
+      <c r="C189" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D189" s="43" t="s">
+        <v>385</v>
+      </c>
+      <c r="E189" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="F189" s="44" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B190" s="42" t="s">
+        <v>402</v>
+      </c>
+      <c r="C190" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D190" s="42" t="s">
+        <v>385</v>
+      </c>
+      <c r="E190" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="F190" s="41" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="43"/>
+      <c r="B191" s="43" t="s">
+        <v>403</v>
+      </c>
+      <c r="C191" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D191" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="E191" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="F191" s="44" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B192" s="42" t="s">
+        <v>404</v>
+      </c>
+      <c r="C192" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D192" s="42" t="s">
+        <v>391</v>
+      </c>
+      <c r="E192" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="F192" s="41" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="43"/>
+      <c r="B193" s="43" t="s">
+        <v>405</v>
+      </c>
+      <c r="C193" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D193" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="E193" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="F193" s="44" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B194" s="42" t="s">
+        <v>406</v>
+      </c>
+      <c r="C194" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D194" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E194" s="45" t="s">
+        <v>372</v>
+      </c>
+      <c r="F194" s="41" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B195" s="42" t="s">
+        <v>407</v>
+      </c>
+      <c r="C195" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D195" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E195" s="45" t="s">
+        <v>408</v>
+      </c>
+      <c r="F195" s="41" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating colors on functional reqs
</commit_message>
<xml_diff>
--- a/functional_reqs.xlsx
+++ b/functional_reqs.xlsx
@@ -1623,7 +1623,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1683,6 +1683,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1698,7 +1704,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1720,7 +1726,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1733,7 +1740,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1743,13 +1749,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
@@ -1760,9 +1771,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF99FF99"/>
       <color rgb="FFEF5F5F"/>
       <color rgb="FFFF99FF"/>
+      <color rgb="FF99FF99"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FF6666FF"/>
@@ -2065,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,30 +2139,30 @@
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="30" t="s">
         <v>364</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="45">
         <v>1</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="E16" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="F16" s="46" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2212,54 +2223,57 @@
         <v>361</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
+    <row r="20" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21">
         <v>5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
+    <row r="21" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
+    <row r="22" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21">
         <v>7</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="21">
         <v>6</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="22" t="s">
         <v>355</v>
       </c>
     </row>
@@ -2317,71 +2331,75 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
+    <row r="26" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21">
         <v>11</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="21">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
+    <row r="27" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="48"/>
+      <c r="B27" s="48">
         <v>12</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="48">
         <v>11</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="47" t="s">
         <v>369</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
+    <row r="28" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="48"/>
+      <c r="B28" s="48">
         <v>13</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="48">
         <v>11</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="47" t="s">
         <v>369</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="49" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
+    <row r="29" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="48"/>
+      <c r="B29" s="48">
         <v>14</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="48">
         <v>11</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="47" t="s">
         <v>369</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="49" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2403,23 +2421,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+    <row r="31" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="26">
         <v>16</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="39" t="s">
         <v>367</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="27" t="s">
         <v>283</v>
       </c>
     </row>
@@ -2617,55 +2635,57 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30">
+    <row r="42" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31">
         <v>26</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="32" t="s">
         <v>370</v>
       </c>
       <c r="F42" s="38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="1">
+    <row r="43" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21">
         <v>27</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="E43" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="1">
+    <row r="44" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21">
         <v>28</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="32" t="s">
+      <c r="E44" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2680,7 +2700,7 @@
       <c r="D45" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="32" t="s">
         <v>371</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -2698,7 +2718,7 @@
       <c r="D46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="32" t="s">
         <v>371</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -2716,7 +2736,7 @@
       <c r="D47" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="32" t="s">
         <v>371</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -2741,23 +2761,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="30">
+    <row r="49" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="31">
         <v>16</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B49" s="29">
         <v>33</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D49" s="30" t="s">
+      <c r="D49" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="32" t="s">
         <v>372</v>
       </c>
-      <c r="F49" s="31" t="s">
+      <c r="F49" s="32" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2781,43 +2801,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27">
+    <row r="51" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="28">
         <v>17</v>
       </c>
-      <c r="B51" s="27">
+      <c r="B51" s="28">
         <v>35</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E51" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="F51" s="31" t="s">
+      <c r="F51" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27">
+    <row r="52" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="28">
         <v>17</v>
       </c>
-      <c r="B52" s="27">
+      <c r="B52" s="28">
         <v>36</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="F52" s="31" t="s">
+      <c r="F52" s="32" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2981,71 +3001,75 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="1">
+    <row r="61" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21">
         <v>45</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="32" t="s">
+      <c r="E61" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="1">
+    <row r="62" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21">
         <v>46</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E62" s="32" t="s">
+      <c r="E62" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="1">
+    <row r="63" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21">
         <v>47</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="1">
+    <row r="64" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21">
         <v>48</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="32" t="s">
+      <c r="E64" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="22" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3149,20 +3173,20 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B70" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="18" t="s">
+      <c r="C70" s="22" t="s">
         <v>60</v>
       </c>
       <c r="D70" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="E70" s="22" t="s">
         <v>365</v>
       </c>
       <c r="F70" s="21" t="s">
@@ -3322,170 +3346,170 @@
       <c r="D78" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E78" s="31" t="s">
+      <c r="E78" s="32" t="s">
         <v>365</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E79" s="32" t="s">
+      <c r="E79" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" s="21" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30" t="s">
+    <row r="80" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B80" s="30" t="s">
+      <c r="B80" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="C80" s="31" t="s">
+      <c r="C80" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D80" s="30" t="s">
+      <c r="D80" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E80" s="31" t="s">
+      <c r="E80" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="F80" s="30" t="s">
+      <c r="F80" s="31" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E81" s="32" t="s">
+      <c r="E81" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F81" s="21" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E82" s="32" t="s">
+      <c r="E82" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="F82" s="21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E83" s="32" t="s">
+      <c r="E83" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="F83" s="21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E84" s="32" t="s">
+      <c r="E84" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="F84" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="30" t="s">
+    <row r="85" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C85" s="31" t="s">
+      <c r="C85" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D85" s="30" t="s">
+      <c r="D85" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="E85" s="31" t="s">
-        <v>365</v>
-      </c>
-      <c r="F85" s="30" t="s">
+      <c r="E85" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="F85" s="31" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="30" t="s">
+    <row r="86" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="B86" s="30" t="s">
+      <c r="B86" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C86" s="31" t="s">
+      <c r="C86" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D86" s="30" t="s">
+      <c r="D86" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="E86" s="31" t="s">
-        <v>365</v>
-      </c>
-      <c r="F86" s="30" t="s">
+      <c r="E86" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="F86" s="31" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4062,7 +4086,7 @@
       <c r="D115" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E115" s="31" t="s">
+      <c r="E115" s="32" t="s">
         <v>365</v>
       </c>
       <c r="F115" s="2" t="s">
@@ -4249,19 +4273,19 @@
         <v>223</v>
       </c>
     </row>
-    <row r="125" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="22"/>
-      <c r="B125" s="22" t="s">
+    <row r="125" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="23"/>
+      <c r="B125" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="C125" s="23" t="s">
+      <c r="C125" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D125" s="22"/>
-      <c r="E125" s="23" t="s">
+      <c r="D125" s="23"/>
+      <c r="E125" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="F125" s="23" t="s">
+      <c r="F125" s="24" t="s">
         <v>296</v>
       </c>
     </row>
@@ -4741,7 +4765,7 @@
       <c r="E152" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="F152" s="31" t="s">
+      <c r="F152" s="32" t="s">
         <v>360</v>
       </c>
     </row>
@@ -4901,35 +4925,35 @@
         <v>311</v>
       </c>
     </row>
-    <row r="162" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="40"/>
-      <c r="B162" s="40" t="s">
+    <row r="162" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="50"/>
+      <c r="B162" s="50" t="s">
         <v>312</v>
       </c>
-      <c r="C162" s="46" t="s">
+      <c r="C162" s="51" t="s">
         <v>299</v>
       </c>
-      <c r="D162" s="40"/>
-      <c r="E162" s="46" t="s">
+      <c r="D162" s="50"/>
+      <c r="E162" s="51" t="s">
         <v>377</v>
       </c>
-      <c r="F162" s="46" t="s">
+      <c r="F162" s="51" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="163" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="40"/>
-      <c r="B163" s="40" t="s">
+    <row r="163" spans="1:6" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="50"/>
+      <c r="B163" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="C163" s="46" t="s">
+      <c r="C163" s="51" t="s">
         <v>299</v>
       </c>
-      <c r="D163" s="40"/>
-      <c r="E163" s="46" t="s">
+      <c r="D163" s="50"/>
+      <c r="E163" s="51" t="s">
         <v>378</v>
       </c>
-      <c r="F163" s="46" t="s">
+      <c r="F163" s="51" t="s">
         <v>328</v>
       </c>
     </row>
@@ -5019,17 +5043,19 @@
         <v>326</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B169" s="1" t="s">
+    <row r="169" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="21"/>
+      <c r="B169" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="E169" s="32" t="s">
+      <c r="D169" s="21"/>
+      <c r="E169" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="F169" t="s">
+      <c r="F169" s="22" t="s">
         <v>329</v>
       </c>
     </row>
@@ -5136,20 +5162,21 @@
         <v>341</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B176" s="1" t="s">
+    <row r="176" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+      <c r="B176" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C176" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D176" s="1" t="s">
+      <c r="D176" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="E176" s="32" t="s">
+      <c r="E176" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F176" s="19" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5162,7 +5189,7 @@
         <v>32</v>
       </c>
       <c r="D177" s="2"/>
-      <c r="E177" s="31" t="s">
+      <c r="E177" s="32" t="s">
         <v>371</v>
       </c>
       <c r="F177" s="3" t="s">
@@ -5178,7 +5205,7 @@
         <v>32</v>
       </c>
       <c r="D178" s="2"/>
-      <c r="E178" s="31" t="s">
+      <c r="E178" s="32" t="s">
         <v>371</v>
       </c>
       <c r="F178" s="3" t="s">
@@ -5194,7 +5221,7 @@
         <v>32</v>
       </c>
       <c r="D179" s="2"/>
-      <c r="E179" s="31" t="s">
+      <c r="E179" s="32" t="s">
         <v>371</v>
       </c>
       <c r="F179" s="3" t="s">
@@ -5210,7 +5237,7 @@
         <v>32</v>
       </c>
       <c r="D180" s="2"/>
-      <c r="E180" s="31" t="s">
+      <c r="E180" s="32" t="s">
         <v>379</v>
       </c>
       <c r="F180" s="3" t="s">
@@ -5235,248 +5262,254 @@
         <v>354</v>
       </c>
     </row>
-    <row r="182" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="21"/>
       <c r="B182" s="21" t="s">
         <v>358</v>
       </c>
-      <c r="C182" s="18" t="s">
+      <c r="C182" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D182" s="21" t="s">
         <v>356</v>
       </c>
-      <c r="E182" s="18" t="s">
+      <c r="E182" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="F182" s="18" t="s">
+      <c r="F182" s="22" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="183" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="30"/>
-      <c r="B183" s="30" t="s">
+    <row r="183" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="31"/>
+      <c r="B183" s="31" t="s">
         <v>362</v>
       </c>
-      <c r="C183" s="31" t="s">
+      <c r="C183" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D183" s="30">
+      <c r="D183" s="31">
         <v>6</v>
       </c>
-      <c r="E183" s="31" t="s">
+      <c r="E183" s="32" t="s">
         <v>370</v>
       </c>
       <c r="F183" s="37" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="184" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="43"/>
-      <c r="B184" s="43" t="s">
+    <row r="184" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="42"/>
+      <c r="B184" s="42" t="s">
         <v>396</v>
       </c>
-      <c r="C184" s="44" t="s">
+      <c r="C184" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D184" s="43" t="s">
+      <c r="D184" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E184" s="44" t="s">
+      <c r="E184" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="F184" s="44" t="s">
+      <c r="F184" s="43" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B185" s="42" t="s">
+      <c r="B185" s="41" t="s">
         <v>397</v>
       </c>
-      <c r="C185" s="41" t="s">
+      <c r="C185" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D185" s="42" t="s">
+      <c r="D185" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E185" s="45" t="s">
+      <c r="E185" s="44" t="s">
         <v>372</v>
       </c>
-      <c r="F185" s="41" t="s">
+      <c r="F185" s="40" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B186" s="42" t="s">
+    <row r="186" spans="1:6" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="45"/>
+      <c r="B186" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="C186" s="41" t="s">
+      <c r="C186" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="D186" s="42" t="s">
+      <c r="D186" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E186" s="45" t="s">
+      <c r="E186" s="46" t="s">
         <v>372</v>
       </c>
-      <c r="F186" s="41" t="s">
+      <c r="F186" s="46" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="187" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="43"/>
-      <c r="B187" s="43" t="s">
+    <row r="187" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="42"/>
+      <c r="B187" s="42" t="s">
         <v>399</v>
       </c>
-      <c r="C187" s="44" t="s">
+      <c r="C187" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D187" s="43" t="s">
+      <c r="D187" s="42" t="s">
         <v>383</v>
       </c>
-      <c r="E187" s="44" t="s">
+      <c r="E187" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="F187" s="44" t="s">
+      <c r="F187" s="43" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B188" s="42" t="s">
+    <row r="188" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="21"/>
+      <c r="B188" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="C188" s="41" t="s">
+      <c r="C188" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D188" s="42" t="s">
+      <c r="D188" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E188" s="45" t="s">
+      <c r="E188" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="F188" s="41" t="s">
+      <c r="F188" s="22" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="189" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="43"/>
-      <c r="B189" s="43" t="s">
+    <row r="189" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="42"/>
+      <c r="B189" s="42" t="s">
         <v>401</v>
       </c>
-      <c r="C189" s="44" t="s">
+      <c r="C189" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D189" s="43" t="s">
+      <c r="D189" s="42" t="s">
         <v>385</v>
       </c>
-      <c r="E189" s="44" t="s">
+      <c r="E189" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="F189" s="44" t="s">
+      <c r="F189" s="43" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B190" s="42" t="s">
+    <row r="190" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="21"/>
+      <c r="B190" s="21" t="s">
         <v>402</v>
       </c>
-      <c r="C190" s="41" t="s">
+      <c r="C190" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D190" s="42" t="s">
+      <c r="D190" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E190" s="45" t="s">
+      <c r="E190" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="F190" s="41" t="s">
+      <c r="F190" s="22" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="191" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="43"/>
-      <c r="B191" s="43" t="s">
+    <row r="191" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="42"/>
+      <c r="B191" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="C191" s="44" t="s">
+      <c r="C191" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D191" s="43" t="s">
+      <c r="D191" s="42" t="s">
         <v>389</v>
       </c>
-      <c r="E191" s="44" t="s">
+      <c r="E191" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="F191" s="44" t="s">
+      <c r="F191" s="43" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B192" s="42" t="s">
+    <row r="192" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="21"/>
+      <c r="B192" s="21" t="s">
         <v>404</v>
       </c>
-      <c r="C192" s="41" t="s">
+      <c r="C192" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D192" s="42" t="s">
+      <c r="D192" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="E192" s="45" t="s">
+      <c r="E192" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="F192" s="41" t="s">
+      <c r="F192" s="22" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="193" spans="1:6" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="43"/>
-      <c r="B193" s="43" t="s">
+    <row r="193" spans="1:6" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="42"/>
+      <c r="B193" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="C193" s="44" t="s">
+      <c r="C193" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D193" s="43" t="s">
+      <c r="D193" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="E193" s="44" t="s">
+      <c r="E193" s="43" t="s">
         <v>372</v>
       </c>
-      <c r="F193" s="44" t="s">
+      <c r="F193" s="43" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B194" s="42" t="s">
+    <row r="194" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="21"/>
+      <c r="B194" s="21" t="s">
         <v>406</v>
       </c>
-      <c r="C194" s="41" t="s">
+      <c r="C194" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D194" s="42" t="s">
+      <c r="D194" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E194" s="45" t="s">
+      <c r="E194" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="F194" s="41" t="s">
+      <c r="F194" s="22" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B195" s="42" t="s">
+    <row r="195" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="21"/>
+      <c r="B195" s="21" t="s">
         <v>407</v>
       </c>
-      <c r="C195" s="41" t="s">
+      <c r="C195" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D195" s="42" t="s">
+      <c r="D195" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E195" s="45" t="s">
+      <c r="E195" s="22" t="s">
         <v>408</v>
       </c>
-      <c r="F195" s="41" t="s">
+      <c r="F195" s="22" t="s">
         <v>395</v>
       </c>
     </row>

</xml_diff>